<commit_message>
update worklog with sunday's stuff
</commit_message>
<xml_diff>
--- a/personal-logs/mitch-harris/WorkLog_mh.xlsx
+++ b/personal-logs/mitch-harris/WorkLog_mh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitch/data_labs/DATA599/w2020-data599-capstone-projects-ubc-udl/personal-logs/mitch-harris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D38D1A6-DE42-B147-9C6E-E3A76E325626}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A2F59E-1C48-6447-9E58-54F9CEB35F1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Master of Data Science Capstone Project - 2021</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Create gantt chart</t>
+  </si>
+  <si>
+    <t>Reseached existant python modules for online anoamly detection</t>
+  </si>
+  <si>
+    <t>Backgorund Review</t>
   </si>
 </sst>
 </file>
@@ -986,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D98CD107-3D4A-C748-A102-5D964726FCA8}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1505,10 +1511,16 @@
       <c r="B68" s="35"/>
       <c r="C68" s="8"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="9"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
+    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="9"/>
@@ -1556,7 +1568,7 @@
       <c r="C78" s="14"/>
       <c r="D78">
         <f>SUM(C69:C78)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -1577,7 +1589,7 @@
       <c r="B81" s="17"/>
       <c r="C81" s="30">
         <f>SUM(C14:C78)</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D81" s="18"/>
     </row>

</xml_diff>

<commit_message>
add mitch work log
</commit_message>
<xml_diff>
--- a/personal-logs/mitch-harris/WorkLog_mh.xlsx
+++ b/personal-logs/mitch-harris/WorkLog_mh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitch/data_labs/DATA599/w2020-data599-capstone-projects-ubc-udl/personal-logs/mitch-harris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862D30FF-F645-F745-A00B-E4B1F9C1DC37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EC4B0D-1CA3-D740-AA80-2E92BC277F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>Master of Data Science Capstone Project - 2021</t>
   </si>
@@ -161,6 +161,45 @@
   </si>
   <si>
     <t>Stand up and presentation run through</t>
+  </si>
+  <si>
+    <t>Data 599 presentation</t>
+  </si>
+  <si>
+    <t>Model &amp; package research</t>
+  </si>
+  <si>
+    <t>Stand up</t>
+  </si>
+  <si>
+    <t>Interal Meetings</t>
+  </si>
+  <si>
+    <t>Model Research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background Research </t>
+  </si>
+  <si>
+    <t>Meeting to figure out Docker</t>
+  </si>
+  <si>
+    <t>Sprint Planning</t>
+  </si>
+  <si>
+    <t>Figure out Docker</t>
+  </si>
+  <si>
+    <t>Infrastructure set up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test different Modeling Frameworks </t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Test different Algorithms for different types of anomalies</t>
   </si>
 </sst>
 </file>
@@ -170,7 +209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,6 +303,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
@@ -510,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -621,14 +666,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -754,12 +791,28 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="6" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="16" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1333,11 +1386,11 @@
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34">
+      <c r="A14" s="70">
         <f>D3</f>
         <v>44319</v>
       </c>
-      <c r="B14" s="35"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1399,11 +1452,11 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34">
+      <c r="A21" s="70">
         <f>A14+1</f>
         <v>44320</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1476,11 +1529,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34">
+      <c r="A29" s="70">
         <f>A21+1</f>
         <v>44321</v>
       </c>
-      <c r="B29" s="35"/>
+      <c r="B29" s="71"/>
       <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1531,11 +1584,11 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34">
+      <c r="A35" s="70">
         <f>A29+1</f>
         <v>44322</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="71"/>
       <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1617,11 +1670,11 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34">
+      <c r="A46" s="70">
         <f>A35+1</f>
         <v>44323</v>
       </c>
-      <c r="B46" s="35"/>
+      <c r="B46" s="71"/>
       <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1691,11 +1744,11 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="34">
+      <c r="A57" s="70">
         <f>A46+1</f>
         <v>44324</v>
       </c>
-      <c r="B57" s="35"/>
+      <c r="B57" s="71"/>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1753,11 +1806,11 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="34">
+      <c r="A68" s="70">
         <f>A57+1</f>
         <v>44325</v>
       </c>
-      <c r="B68" s="35"/>
+      <c r="B68" s="71"/>
       <c r="C68" s="8"/>
     </row>
     <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2013,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27588B11-1EF5-1D41-B8BD-E638D371F0AF}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2031,69 +2084,69 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="36"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="37"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="35"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="39">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="37">
         <v>44326</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="42">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="35"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="37"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="35"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
@@ -2101,129 +2154,129 @@
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="37"/>
+      <c r="D10" s="35"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="37"/>
+      <c r="D11" s="35"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
     </row>
     <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="46"/>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34">
+      <c r="A14" s="70">
         <v>44326</v>
       </c>
-      <c r="B14" s="35"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="37"/>
+      <c r="D14" s="35"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="46">
         <v>6</v>
       </c>
-      <c r="D15" s="37"/>
+      <c r="D15" s="35"/>
     </row>
     <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.2">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="49">
         <v>0.25</v>
       </c>
-      <c r="D16" s="37"/>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="46">
         <v>1.5</v>
       </c>
-      <c r="D17" s="37"/>
+      <c r="D17" s="35"/>
     </row>
     <row r="18" spans="1:4" ht="71" x14ac:dyDescent="0.2">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="51">
+      <c r="C18" s="49">
         <v>1.25</v>
       </c>
-      <c r="D18" s="37"/>
+      <c r="D18" s="35"/>
     </row>
     <row r="19" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="53">
+      <c r="C19" s="51">
         <v>0.5</v>
       </c>
-      <c r="D19" s="37"/>
+      <c r="D19" s="35"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="54"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="37"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="35"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="57"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="37"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="35"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="59"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="37"/>
+      <c r="A22" s="57"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="35"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="57"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="37"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="35"/>
     </row>
     <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="37">
+      <c r="A24" s="57"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="35">
         <f>SUM(C15:C24)</f>
         <v>9.5</v>
       </c>
@@ -2234,151 +2287,176 @@
       </c>
       <c r="B25" s="73"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="37"/>
+      <c r="D25" s="35"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="51">
+      <c r="C26" s="49">
         <v>1</v>
       </c>
-      <c r="D26" s="37"/>
+      <c r="D26" s="35"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="48">
+      <c r="C27" s="46">
         <v>0.75</v>
       </c>
-      <c r="D27" s="37"/>
+      <c r="D27" s="35"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="37"/>
+      <c r="A28" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="35"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="47"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="37"/>
+      <c r="A29" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="46">
+        <v>5</v>
+      </c>
+      <c r="D29" s="35"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="49"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="37"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="35"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="47"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="37"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="35"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="49"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="37"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="35"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="57"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="37"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="35"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="59"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="37"/>
+      <c r="A34" s="57"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="35"/>
     </row>
     <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="57"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="37">
+      <c r="A35" s="55"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="35">
         <f>SUM(C26:C35)</f>
-        <v>1.75</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="34">
+      <c r="A36" s="70">
         <v>44328</v>
       </c>
-      <c r="B36" s="35"/>
+      <c r="B36" s="71"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="37"/>
+      <c r="D36" s="35"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="47"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="37"/>
+      <c r="A37" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="35"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="49"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="37"/>
+      <c r="A38" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="49">
+        <v>6</v>
+      </c>
+      <c r="D38" s="35"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="47"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="37"/>
+      <c r="A39" s="45"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="35"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="49"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="37"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="35"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="47"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="62"/>
+      <c r="A41" s="45"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="60"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="49"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="37"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="35"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="52"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="62"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="60"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="54"/>
-      <c r="B44" s="55"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="37"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="35"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="57"/>
-      <c r="B45" s="58"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="37"/>
+      <c r="A45" s="55"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="35"/>
     </row>
     <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="59"/>
-      <c r="B46" s="60"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="37">
-        <v>0</v>
+      <c r="A46" s="57"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="35">
+        <f>SUM(C37:C46)</f>
+        <v>6.5</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2387,138 +2465,182 @@
       </c>
       <c r="B47" s="73"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="37"/>
+      <c r="D47" s="35"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="49"/>
-      <c r="B48" s="50"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="37"/>
+      <c r="A48" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D48" s="35"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="47"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="37"/>
+      <c r="A49" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="35"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="49"/>
-      <c r="B50" s="50"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="37"/>
+      <c r="A50" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="49">
+        <v>1</v>
+      </c>
+      <c r="D50" s="35"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="47"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="48"/>
-      <c r="D51" s="37"/>
+      <c r="A51" s="75" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="46">
+        <v>6</v>
+      </c>
+      <c r="D51" s="35"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="49"/>
-      <c r="B52" s="50"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="37"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="35"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="47"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="37"/>
+      <c r="A53" s="45"/>
+      <c r="B53" s="46"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="35"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="49"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="37"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="35"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="57"/>
-      <c r="B55" s="58"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="37"/>
+      <c r="A55" s="55"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="35"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="59"/>
-      <c r="B56" s="60"/>
-      <c r="C56" s="61"/>
-      <c r="D56" s="37"/>
+      <c r="A56" s="57"/>
+      <c r="B56" s="58"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="35"/>
     </row>
     <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="57"/>
-      <c r="B57" s="58"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="37">
-        <v>0</v>
+      <c r="A57" s="55"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="35">
+        <f>SUM(C48:C57)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="34">
+      <c r="A58" s="70">
         <v>44330</v>
       </c>
-      <c r="B58" s="35"/>
+      <c r="B58" s="71"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="37"/>
+      <c r="D58" s="35"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="47"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="37"/>
+      <c r="A59" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="D59" s="35"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="49"/>
-      <c r="B60" s="50"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="37"/>
+      <c r="A60" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" s="49">
+        <v>3</v>
+      </c>
+      <c r="D60" s="35"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="47"/>
-      <c r="B61" s="48"/>
-      <c r="C61" s="48"/>
-      <c r="D61" s="37"/>
+      <c r="A61" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B61" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" s="46">
+        <v>3</v>
+      </c>
+      <c r="D61" s="35"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="49"/>
-      <c r="B62" s="50"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="37"/>
+      <c r="A62" s="47"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="35"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="47"/>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="37"/>
+      <c r="A63" s="45"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="35"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="49"/>
-      <c r="B64" s="50"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="37"/>
+      <c r="A64" s="47"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="35"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="52"/>
-      <c r="B65" s="53"/>
-      <c r="C65" s="53"/>
-      <c r="D65" s="37"/>
+      <c r="A65" s="50"/>
+      <c r="B65" s="51"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="35"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="54"/>
-      <c r="B66" s="55"/>
-      <c r="C66" s="56"/>
-      <c r="D66" s="37"/>
+      <c r="A66" s="52"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="35"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="57"/>
-      <c r="B67" s="58"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="37"/>
+      <c r="A67" s="55"/>
+      <c r="B67" s="56"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="35"/>
     </row>
     <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="59"/>
-      <c r="B68" s="60"/>
-      <c r="C68" s="61"/>
-      <c r="D68" s="37">
-        <v>0</v>
+      <c r="A68" s="57"/>
+      <c r="B68" s="58"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="35">
+        <f>SUM(C59:C68)</f>
+        <v>6.5</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2527,212 +2649,214 @@
       </c>
       <c r="B69" s="73"/>
       <c r="C69" s="8"/>
-      <c r="D69" s="37"/>
+      <c r="D69" s="35"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="49"/>
-      <c r="B70" s="50"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="37"/>
+      <c r="A70" s="47"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="49"/>
+      <c r="D70" s="35"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="47"/>
-      <c r="B71" s="48"/>
-      <c r="C71" s="48"/>
-      <c r="D71" s="37"/>
+      <c r="A71" s="45"/>
+      <c r="B71" s="46"/>
+      <c r="C71" s="46"/>
+      <c r="D71" s="35"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="49"/>
-      <c r="B72" s="50"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="37"/>
+      <c r="A72" s="47"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="35"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="47"/>
-      <c r="B73" s="48"/>
-      <c r="C73" s="48"/>
-      <c r="D73" s="37"/>
+      <c r="A73" s="45"/>
+      <c r="B73" s="46"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="35"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="49"/>
-      <c r="B74" s="50"/>
-      <c r="C74" s="51"/>
-      <c r="D74" s="37"/>
+      <c r="A74" s="47"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="35"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="47"/>
-      <c r="B75" s="48"/>
-      <c r="C75" s="48"/>
-      <c r="D75" s="37"/>
+      <c r="A75" s="45"/>
+      <c r="B75" s="46"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="35"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="49"/>
-      <c r="B76" s="50"/>
-      <c r="C76" s="51"/>
-      <c r="D76" s="37"/>
+      <c r="A76" s="47"/>
+      <c r="B76" s="48"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="35"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="57"/>
-      <c r="B77" s="58"/>
-      <c r="C77" s="58"/>
-      <c r="D77" s="37"/>
+      <c r="A77" s="55"/>
+      <c r="B77" s="56"/>
+      <c r="C77" s="56"/>
+      <c r="D77" s="35"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="59"/>
-      <c r="B78" s="60"/>
-      <c r="C78" s="61"/>
-      <c r="D78" s="37"/>
+      <c r="A78" s="57"/>
+      <c r="B78" s="58"/>
+      <c r="C78" s="59"/>
+      <c r="D78" s="35"/>
     </row>
     <row r="79" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="57"/>
-      <c r="B79" s="58"/>
-      <c r="C79" s="58"/>
-      <c r="D79" s="37">
+      <c r="A79" s="55"/>
+      <c r="B79" s="56"/>
+      <c r="C79" s="56"/>
+      <c r="D79" s="35">
+        <f>SUM(C70:C79)</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="34">
+      <c r="A80" s="70">
         <v>44332</v>
       </c>
-      <c r="B80" s="35"/>
+      <c r="B80" s="71"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="37"/>
+      <c r="D80" s="35"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="47"/>
-      <c r="B81" s="48"/>
-      <c r="C81" s="48"/>
-      <c r="D81" s="37"/>
+      <c r="A81" s="45"/>
+      <c r="B81" s="46"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="35"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="49"/>
-      <c r="B82" s="50"/>
-      <c r="C82" s="51"/>
-      <c r="D82" s="37"/>
+      <c r="A82" s="47"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="35"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="47"/>
-      <c r="B83" s="48"/>
-      <c r="C83" s="48"/>
-      <c r="D83" s="37"/>
+      <c r="A83" s="45"/>
+      <c r="B83" s="46"/>
+      <c r="C83" s="46"/>
+      <c r="D83" s="35"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="49"/>
-      <c r="B84" s="50"/>
-      <c r="C84" s="51"/>
-      <c r="D84" s="37"/>
+      <c r="A84" s="47"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="35"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="47"/>
-      <c r="B85" s="48"/>
-      <c r="C85" s="48"/>
-      <c r="D85" s="37"/>
+      <c r="A85" s="45"/>
+      <c r="B85" s="46"/>
+      <c r="C85" s="46"/>
+      <c r="D85" s="35"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="49"/>
-      <c r="B86" s="50"/>
-      <c r="C86" s="51"/>
-      <c r="D86" s="37"/>
+      <c r="A86" s="47"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="35"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="52"/>
-      <c r="B87" s="53"/>
-      <c r="C87" s="53"/>
-      <c r="D87" s="37"/>
+      <c r="A87" s="50"/>
+      <c r="B87" s="51"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="35"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="54"/>
-      <c r="B88" s="55"/>
-      <c r="C88" s="56"/>
-      <c r="D88" s="37"/>
+      <c r="A88" s="52"/>
+      <c r="B88" s="53"/>
+      <c r="C88" s="54"/>
+      <c r="D88" s="35"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="57"/>
-      <c r="B89" s="58"/>
-      <c r="C89" s="58"/>
-      <c r="D89" s="37"/>
+      <c r="A89" s="55"/>
+      <c r="B89" s="56"/>
+      <c r="C89" s="56"/>
+      <c r="D89" s="35"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="59"/>
-      <c r="B90" s="60"/>
-      <c r="C90" s="61"/>
-      <c r="D90" s="37">
+      <c r="A90" s="57"/>
+      <c r="B90" s="58"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="35">
+        <f>SUM(C81:C90)</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="63"/>
-      <c r="B91" s="63"/>
-      <c r="C91" s="63"/>
-      <c r="D91" s="37"/>
+      <c r="A91" s="61"/>
+      <c r="B91" s="61"/>
+      <c r="C91" s="61"/>
+      <c r="D91" s="35"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="64"/>
-      <c r="B92" s="65"/>
-      <c r="C92" s="65"/>
-      <c r="D92" s="66"/>
+      <c r="A92" s="62"/>
+      <c r="B92" s="63"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="64"/>
     </row>
     <row r="93" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B93" s="17"/>
-      <c r="C93" s="67">
+      <c r="C93" s="65">
         <f>SUM(D24:D90)</f>
-        <v>11.25</v>
-      </c>
-      <c r="D93" s="68"/>
+        <v>37.75</v>
+      </c>
+      <c r="D93" s="66"/>
     </row>
     <row r="94" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="69"/>
-      <c r="B94" s="70"/>
-      <c r="C94" s="70"/>
-      <c r="D94" s="37"/>
+      <c r="A94" s="67"/>
+      <c r="B94" s="68"/>
+      <c r="C94" s="68"/>
+      <c r="D94" s="35"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="64" t="s">
+      <c r="A95" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="B95" s="65"/>
-      <c r="C95" s="65"/>
+      <c r="B95" s="63"/>
+      <c r="C95" s="63"/>
       <c r="D95" s="21"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="71"/>
+      <c r="A96" s="69"/>
       <c r="B96" s="23"/>
       <c r="C96" s="23"/>
-      <c r="D96" s="37"/>
+      <c r="D96" s="35"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="71"/>
+      <c r="A97" s="69"/>
       <c r="B97" s="23"/>
       <c r="C97" s="23"/>
-      <c r="D97" s="37"/>
+      <c r="D97" s="35"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="69"/>
-      <c r="B98" s="70"/>
-      <c r="C98" s="70"/>
-      <c r="D98" s="37"/>
+      <c r="A98" s="67"/>
+      <c r="B98" s="68"/>
+      <c r="C98" s="68"/>
+      <c r="D98" s="35"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="24"/>
       <c r="B99" s="24"/>
       <c r="C99" s="24"/>
-      <c r="D99" s="37"/>
+      <c r="D99" s="35"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="37"/>
-      <c r="B100" s="37"/>
-      <c r="C100" s="37"/>
-      <c r="D100" s="37"/>
+      <c r="A100" s="35"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="21"/>
-      <c r="D101" s="37"/>
+      <c r="D101" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
update week 3 hours
</commit_message>
<xml_diff>
--- a/personal-logs/mitch-harris/WorkLog_mh.xlsx
+++ b/personal-logs/mitch-harris/WorkLog_mh.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitch/data_labs/DATA599/w2020-data599-capstone-projects-ubc-udl/personal-logs/mitch-harris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EC4B0D-1CA3-D740-AA80-2E92BC277F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08F09D3-A9C1-1847-9FA4-DB375B8F19C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="2" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
     <sheet name="Week 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Week 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="67">
   <si>
     <t>Master of Data Science Capstone Project - 2021</t>
   </si>
@@ -200,6 +201,42 @@
   </si>
   <si>
     <t>Test different Algorithms for different types of anomalies</t>
+  </si>
+  <si>
+    <t>Meeting with UDL</t>
+  </si>
+  <si>
+    <t>Work on power point for presentation</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t>LSTM research and demo</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Meeting with UDL and EWS</t>
+  </si>
+  <si>
+    <t>Meeting with Captstone Advisor</t>
+  </si>
+  <si>
+    <t>Advisor Meeting</t>
+  </si>
+  <si>
+    <t>Advisor Follow up meeting</t>
+  </si>
+  <si>
+    <t>Work on labeling data</t>
+  </si>
+  <si>
+    <t>Model Pipeline Architecture</t>
+  </si>
+  <si>
+    <t>Build Flask App for serving models</t>
   </si>
 </sst>
 </file>
@@ -555,7 +592,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -791,6 +828,14 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -807,11 +852,7 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
@@ -1386,11 +1427,11 @@
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="70">
+      <c r="A14" s="72">
         <f>D3</f>
         <v>44319</v>
       </c>
-      <c r="B14" s="71"/>
+      <c r="B14" s="73"/>
       <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1452,11 +1493,11 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="70">
+      <c r="A21" s="72">
         <f>A14+1</f>
         <v>44320</v>
       </c>
-      <c r="B21" s="71"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1529,11 +1570,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="70">
+      <c r="A29" s="72">
         <f>A21+1</f>
         <v>44321</v>
       </c>
-      <c r="B29" s="71"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1584,11 +1625,11 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="70">
+      <c r="A35" s="72">
         <f>A29+1</f>
         <v>44322</v>
       </c>
-      <c r="B35" s="71"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1670,11 +1711,11 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="70">
+      <c r="A46" s="72">
         <f>A35+1</f>
         <v>44323</v>
       </c>
-      <c r="B46" s="71"/>
+      <c r="B46" s="73"/>
       <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1744,11 +1785,11 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="70">
+      <c r="A57" s="72">
         <f>A46+1</f>
         <v>44324</v>
       </c>
-      <c r="B57" s="71"/>
+      <c r="B57" s="73"/>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1806,11 +1847,11 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="70">
+      <c r="A68" s="72">
         <f>A57+1</f>
         <v>44325</v>
       </c>
-      <c r="B68" s="71"/>
+      <c r="B68" s="73"/>
       <c r="C68" s="8"/>
     </row>
     <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2066,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27588B11-1EF5-1D41-B8BD-E638D371F0AF}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B64" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2181,10 +2222,10 @@
       <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="70">
+      <c r="A14" s="72">
         <v>44326</v>
       </c>
-      <c r="B14" s="71"/>
+      <c r="B14" s="73"/>
       <c r="C14" s="8"/>
       <c r="D14" s="35"/>
     </row>
@@ -2282,10 +2323,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="72">
+      <c r="A25" s="74">
         <v>44327</v>
       </c>
-      <c r="B25" s="73"/>
+      <c r="B25" s="75"/>
       <c r="C25" s="8"/>
       <c r="D25" s="35"/>
     </row>
@@ -2377,10 +2418,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="70">
+      <c r="A36" s="72">
         <v>44328</v>
       </c>
-      <c r="B36" s="71"/>
+      <c r="B36" s="73"/>
       <c r="C36" s="8"/>
       <c r="D36" s="35"/>
     </row>
@@ -2397,7 +2438,7 @@
       <c r="D37" s="35"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="74" t="s">
+      <c r="A38" s="70" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="48" t="s">
@@ -2460,10 +2501,10 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="72">
+      <c r="A47" s="74">
         <v>44329</v>
       </c>
-      <c r="B47" s="73"/>
+      <c r="B47" s="75"/>
       <c r="C47" s="8"/>
       <c r="D47" s="35"/>
     </row>
@@ -2504,7 +2545,7 @@
       <c r="D50" s="35"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="75" t="s">
+      <c r="A51" s="71" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="46" t="s">
@@ -2555,10 +2596,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="70">
+      <c r="A58" s="72">
         <v>44330</v>
       </c>
-      <c r="B58" s="71"/>
+      <c r="B58" s="73"/>
       <c r="C58" s="8"/>
       <c r="D58" s="35"/>
     </row>
@@ -2644,10 +2685,10 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="72">
+      <c r="A69" s="74">
         <v>44331</v>
       </c>
-      <c r="B69" s="73"/>
+      <c r="B69" s="75"/>
       <c r="C69" s="8"/>
       <c r="D69" s="35"/>
     </row>
@@ -2715,10 +2756,10 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="70">
+      <c r="A80" s="72">
         <v>44332</v>
       </c>
-      <c r="B80" s="71"/>
+      <c r="B80" s="73"/>
       <c r="C80" s="8"/>
       <c r="D80" s="35"/>
     </row>
@@ -2805,6 +2846,834 @@
       <c r="C93" s="65">
         <f>SUM(D24:D90)</f>
         <v>37.75</v>
+      </c>
+      <c r="D93" s="66"/>
+    </row>
+    <row r="94" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="67"/>
+      <c r="B94" s="68"/>
+      <c r="C94" s="68"/>
+      <c r="D94" s="35"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" s="63"/>
+      <c r="C95" s="63"/>
+      <c r="D95" s="21"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="69"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="35"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="69"/>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="35"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="67"/>
+      <c r="B98" s="68"/>
+      <c r="C98" s="68"/>
+      <c r="D98" s="35"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="24"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="35"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="35"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="21"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A69:B69"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0723633-256C-754A-A65B-B9FB88256DFB}">
+  <dimension ref="A1:D101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="37">
+        <v>44333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="35"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="35"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="35"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="44"/>
+    </row>
+    <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="72">
+        <v>44333</v>
+      </c>
+      <c r="B14" s="73"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="35"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="46">
+        <v>3</v>
+      </c>
+      <c r="D15" s="35"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="35"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="46">
+        <v>2</v>
+      </c>
+      <c r="D17" s="35"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="49">
+        <v>1</v>
+      </c>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="50"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="55"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="57"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="35"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="55"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="35"/>
+    </row>
+    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="57"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="35">
+        <f>SUM(C15:C24)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="74">
+        <v>44334</v>
+      </c>
+      <c r="B25" s="75"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="49">
+        <v>1</v>
+      </c>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="46">
+        <v>0.75</v>
+      </c>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="49">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="D28" s="35"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="46">
+        <v>4</v>
+      </c>
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="47"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="45"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="35"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="47"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="35"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="55"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="35"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="57"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="35"/>
+    </row>
+    <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="55"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="35">
+        <f>SUM(C26:C35)</f>
+        <v>6.4169999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="72">
+        <v>44335</v>
+      </c>
+      <c r="B36" s="73"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="35"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="35"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="49">
+        <v>5.5</v>
+      </c>
+      <c r="D38" s="35"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="45"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="35"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="47"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="35"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="45"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="60"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="35"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="50"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="60"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="52"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="35"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="55"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="35"/>
+    </row>
+    <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="57"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="35">
+        <f>SUM(C37:C46)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="74">
+        <v>44336</v>
+      </c>
+      <c r="B47" s="75"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="35"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="49">
+        <v>1</v>
+      </c>
+      <c r="D48" s="35"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="46">
+        <v>6</v>
+      </c>
+      <c r="D49" s="35"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="49">
+        <v>1</v>
+      </c>
+      <c r="D50" s="35"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="71"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="35"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="47"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="35"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="45"/>
+      <c r="B53" s="46"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="35"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="47"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="35"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="55"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="35"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="57"/>
+      <c r="B56" s="58"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="35"/>
+    </row>
+    <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="55"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="35">
+        <f>SUM(C48:C57)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="72">
+        <v>44337</v>
+      </c>
+      <c r="B58" s="73"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="35"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="D59" s="35"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="49">
+        <v>1</v>
+      </c>
+      <c r="D60" s="35"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="46">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="D61" s="35"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="49">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D62" s="35"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" s="46">
+        <v>1</v>
+      </c>
+      <c r="D63" s="35"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C64" s="49">
+        <v>3</v>
+      </c>
+      <c r="D64" s="35"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="50"/>
+      <c r="B65" s="51"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="35"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="52"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="35"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="55"/>
+      <c r="B67" s="56"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="35"/>
+    </row>
+    <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="57"/>
+      <c r="B68" s="58"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="35">
+        <f>SUM(C59:C68)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="74">
+        <v>44338</v>
+      </c>
+      <c r="B69" s="75"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="35"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C70" s="49">
+        <v>2</v>
+      </c>
+      <c r="D70" s="35"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="45"/>
+      <c r="B71" s="46"/>
+      <c r="C71" s="46"/>
+      <c r="D71" s="35"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="47"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="35"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="45"/>
+      <c r="B73" s="46"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="35"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="47"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="35"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="45"/>
+      <c r="B75" s="46"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="35"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="47"/>
+      <c r="B76" s="48"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="35"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="55"/>
+      <c r="B77" s="56"/>
+      <c r="C77" s="56"/>
+      <c r="D77" s="35"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="57"/>
+      <c r="B78" s="58"/>
+      <c r="C78" s="59"/>
+      <c r="D78" s="35"/>
+    </row>
+    <row r="79" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="55"/>
+      <c r="B79" s="56"/>
+      <c r="C79" s="56"/>
+      <c r="D79" s="35">
+        <f>SUM(C70:C79)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="72">
+        <v>44339</v>
+      </c>
+      <c r="B80" s="73"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="35"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B81" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C81" s="46">
+        <v>5</v>
+      </c>
+      <c r="D81" s="35"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="47"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="35"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="45"/>
+      <c r="B83" s="46"/>
+      <c r="C83" s="46"/>
+      <c r="D83" s="35"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="47"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="35"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="45"/>
+      <c r="B85" s="46"/>
+      <c r="C85" s="46"/>
+      <c r="D85" s="35"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="47"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="35"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="50"/>
+      <c r="B87" s="51"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="35"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="52"/>
+      <c r="B88" s="53"/>
+      <c r="C88" s="54"/>
+      <c r="D88" s="35"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="55"/>
+      <c r="B89" s="56"/>
+      <c r="C89" s="56"/>
+      <c r="D89" s="35"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="57"/>
+      <c r="B90" s="58"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="35">
+        <f>SUM(C81:C90)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="61"/>
+      <c r="B91" s="61"/>
+      <c r="C91" s="61"/>
+      <c r="D91" s="35"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="62"/>
+      <c r="B92" s="63"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="64"/>
+    </row>
+    <row r="93" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93" s="17"/>
+      <c r="C93" s="65">
+        <f>SUM(D24:D90)</f>
+        <v>40.417000000000002</v>
       </c>
       <c r="D93" s="66"/>
     </row>

</xml_diff>

<commit_message>
update logs, add weekly-summary.xlsx
</commit_message>
<xml_diff>
--- a/personal-logs/mitch-harris/WorkLog_mh.xlsx
+++ b/personal-logs/mitch-harris/WorkLog_mh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitch/data_labs/DATA599/w2020-data599-capstone-projects-ubc-udl/personal-logs/mitch-harris/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\MDS\capstone\w2020-data599-capstone-projects-ubc-udl\personal-logs\mitch-harris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08F09D3-A9C1-1847-9FA4-DB375B8F19C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D55D6B-1EAC-43F2-8743-EF523E562E42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="2" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -22,21 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="65">
   <si>
     <t>Master of Data Science Capstone Project - 2021</t>
   </si>
@@ -149,9 +140,6 @@
     <t>Post-meeting internal discussion</t>
   </si>
   <si>
-    <t>Parsing Files</t>
-  </si>
-  <si>
     <t>Anomaly Decection Package Research</t>
   </si>
   <si>
@@ -209,24 +197,15 @@
     <t>Work on power point for presentation</t>
   </si>
   <si>
-    <t>Reporting</t>
-  </si>
-  <si>
     <t>LSTM research and demo</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Meeting with UDL and EWS</t>
   </si>
   <si>
     <t>Meeting with Captstone Advisor</t>
   </si>
   <si>
-    <t>Advisor Meeting</t>
-  </si>
-  <si>
     <t>Advisor Follow up meeting</t>
   </si>
   <si>
@@ -237,6 +216,12 @@
   </si>
   <si>
     <t>Build Flask App for serving models</t>
+  </si>
+  <si>
+    <t>Software Setup</t>
+  </si>
+  <si>
+    <t>Model Selection</t>
   </si>
 </sst>
 </file>
@@ -836,6 +821,10 @@
       <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -850,10 +839,6 @@
     </xf>
     <xf numFmtId="16" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -861,7 +846,14 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1335,19 +1327,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D98CD107-3D4A-C748-A102-5D964726FCA8}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="7.5" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="59" customWidth="1"/>
     <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.296875" customWidth="1"/>
+    <col min="4" max="4" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -1355,17 +1347,17 @@
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D3" s="31">
         <v>44319</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1383,38 +1375,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
@@ -1426,15 +1418,15 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72">
+    <row r="14" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="73">
         <f>D3</f>
         <v>44319</v>
       </c>
-      <c r="B14" s="73"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
@@ -1445,7 +1437,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>11</v>
       </c>
@@ -1456,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>13</v>
       </c>
@@ -1467,7 +1459,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>14</v>
       </c>
@@ -1478,12 +1470,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
     </row>
-    <row r="20" spans="1:4" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -1492,15 +1484,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="72">
+    <row r="21" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="73">
         <f>A14+1</f>
         <v>44320</v>
       </c>
-      <c r="B21" s="73"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>16</v>
       </c>
@@ -1511,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>17</v>
       </c>
@@ -1522,7 +1514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>31</v>
       </c>
@@ -1533,7 +1525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>19</v>
       </c>
@@ -1544,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>21</v>
       </c>
@@ -1555,12 +1547,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
     </row>
-    <row r="28" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -1569,15 +1561,15 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="72">
+    <row r="29" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="73">
         <f>A21+1</f>
         <v>44321</v>
       </c>
-      <c r="B29" s="73"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>30</v>
       </c>
@@ -1588,7 +1580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>22</v>
       </c>
@@ -1599,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>13</v>
       </c>
@@ -1610,12 +1602,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
     </row>
-    <row r="34" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -1624,15 +1616,15 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="72">
+    <row r="35" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="73">
         <f>A29+1</f>
         <v>44322</v>
       </c>
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="8"/>
     </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>30</v>
       </c>
@@ -1643,7 +1635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>23</v>
       </c>
@@ -1654,7 +1646,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>24</v>
       </c>
@@ -1665,7 +1657,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>25</v>
       </c>
@@ -1676,32 +1668,32 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="32"/>
       <c r="B40" s="32"/>
       <c r="C40" s="32"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="33"/>
       <c r="B41" s="33"/>
       <c r="C41" s="33"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="11"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
     </row>
-    <row r="45" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="13"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -1710,26 +1702,26 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="72">
+    <row r="46" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="73">
         <f>A35+1</f>
         <v>44323</v>
       </c>
-      <c r="B46" s="73"/>
+      <c r="B46" s="74"/>
       <c r="C46" s="8"/>
     </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C47" s="10">
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>30</v>
       </c>
@@ -1740,42 +1732,42 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="9"/>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="9"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="11"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
     </row>
-    <row r="56" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="13"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -1784,60 +1776,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="72">
+    <row r="57" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="73">
         <f>A46+1</f>
         <v>44324</v>
       </c>
-      <c r="B57" s="73"/>
+      <c r="B57" s="74"/>
       <c r="C57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="9"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="9"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="11"/>
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="13"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="13"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
     </row>
-    <row r="67" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="13"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
@@ -1846,15 +1838,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="72">
+    <row r="68" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="73">
         <f>A57+1</f>
         <v>44325</v>
       </c>
-      <c r="B68" s="73"/>
+      <c r="B68" s="74"/>
       <c r="C68" s="8"/>
     </row>
-    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
         <v>32</v>
       </c>
@@ -1865,47 +1857,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="9"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="9"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="9"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="11"/>
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="13"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="13"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="13"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
@@ -1914,18 +1906,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="15"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A80" s="28"/>
       <c r="B80" s="29"/>
       <c r="C80" s="29"/>
       <c r="D80" s="16"/>
     </row>
-    <row r="81" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="17" t="s">
         <v>27</v>
       </c>
@@ -1936,12 +1928,12 @@
       </c>
       <c r="D81" s="18"/>
     </row>
-    <row r="82" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A82" s="19"/>
       <c r="B82" s="20"/>
       <c r="C82" s="20"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A83" s="28" t="s">
         <v>28</v>
       </c>
@@ -1949,27 +1941,27 @@
       <c r="C83" s="29"/>
       <c r="D83" s="21"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="22"/>
       <c r="B84" s="23"/>
       <c r="C84" s="23"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="22"/>
       <c r="B85" s="23"/>
       <c r="C85" s="23"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="19"/>
       <c r="B86" s="20"/>
       <c r="C86" s="20"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A87" s="24"/>
       <c r="B87" s="24"/>
       <c r="C87" s="24"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A89" s="21"/>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
@@ -1985,112 +1977,107 @@
     <mergeCell ref="A57:B57"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A15:C20 A30:C34 A22:C28 A42:C45 A36:C39">
+    <cfRule type="expression" dxfId="23" priority="28" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
     <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="21" priority="26" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B33">
-    <cfRule type="expression" dxfId="19" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C52">
-    <cfRule type="expression" dxfId="18" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C56">
-    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B56 A47">
+    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:B52 A47">
     <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48:B52 A47">
-    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
+  <conditionalFormatting sqref="A58:B67">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A58:B67">
+  <conditionalFormatting sqref="A58:B63">
     <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A58:B63">
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C58:C63">
-    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C67">
-    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B78">
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C74">
-    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C78">
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B74">
-    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
+    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
     <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2107,19 +2094,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27588B11-1EF5-1D41-B8BD-E638D371F0AF}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B64" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C51" activeCellId="1" sqref="C17 C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.1640625" customWidth="1"/>
+    <col min="1" max="1" width="53.19921875" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -2127,13 +2114,13 @@
       <c r="C1" s="1"/>
       <c r="D1" s="34"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="36"/>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A3" s="35"/>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
@@ -2141,7 +2128,7 @@
         <v>44326</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="s">
         <v>0</v>
       </c>
@@ -2151,7 +2138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>2</v>
       </c>
@@ -2161,7 +2148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
@@ -2169,19 +2156,19 @@
       <c r="C6" s="38"/>
       <c r="D6" s="35"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A7" s="38"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
       <c r="D7" s="35"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A8" s="35"/>
       <c r="B8" s="35"/>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A9" s="41" t="s">
         <v>4</v>
       </c>
@@ -2189,7 +2176,7 @@
       <c r="C9" s="42"/>
       <c r="D9" s="35"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -2197,19 +2184,19 @@
       <c r="C10" s="6"/>
       <c r="D10" s="35"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="35"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A12" s="35"/>
       <c r="B12" s="35"/>
       <c r="C12" s="35"/>
       <c r="D12" s="35"/>
     </row>
-    <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="43" t="s">
         <v>6</v>
       </c>
@@ -2221,17 +2208,17 @@
       </c>
       <c r="D13" s="44"/>
     </row>
-    <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72">
+    <row r="14" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="73">
         <v>44326</v>
       </c>
-      <c r="B14" s="73"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="8"/>
       <c r="D14" s="35"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A15" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="46" t="s">
         <v>16</v>
@@ -2241,7 +2228,7 @@
       </c>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A16" s="47" t="s">
         <v>34</v>
       </c>
@@ -2253,19 +2240,19 @@
       </c>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C17" s="46">
         <v>1.5</v>
       </c>
       <c r="D17" s="35"/>
     </row>
-    <row r="18" spans="1:4" ht="71" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A18" s="47" t="s">
         <v>35</v>
       </c>
@@ -2277,7 +2264,7 @@
       </c>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A19" s="50" t="s">
         <v>36</v>
       </c>
@@ -2289,31 +2276,31 @@
       </c>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A20" s="52"/>
       <c r="B20" s="53"/>
       <c r="C20" s="54"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A21" s="55"/>
       <c r="B21" s="56"/>
       <c r="C21" s="56"/>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A22" s="57"/>
       <c r="B22" s="58"/>
       <c r="C22" s="59"/>
       <c r="D22" s="35"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A23" s="55"/>
       <c r="B23" s="56"/>
       <c r="C23" s="56"/>
       <c r="D23" s="35"/>
     </row>
-    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="57"/>
       <c r="B24" s="58"/>
       <c r="C24" s="59"/>
@@ -2322,17 +2309,17 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="74">
+    <row r="25" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="75">
         <v>44327</v>
       </c>
-      <c r="B25" s="75"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="8"/>
       <c r="D25" s="35"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A26" s="47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="48" t="s">
         <v>16</v>
@@ -2342,9 +2329,9 @@
       </c>
       <c r="D26" s="35"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A27" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>10</v>
@@ -2354,9 +2341,9 @@
       </c>
       <c r="D27" s="35"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A28" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>10</v>
@@ -2366,9 +2353,9 @@
       </c>
       <c r="D28" s="35"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A29" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="46" t="s">
         <v>16</v>
@@ -2378,37 +2365,37 @@
       </c>
       <c r="D29" s="35"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A30" s="47"/>
       <c r="B30" s="48"/>
       <c r="C30" s="49"/>
       <c r="D30" s="35"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A31" s="45"/>
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
       <c r="D31" s="35"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A32" s="47"/>
       <c r="B32" s="48"/>
       <c r="C32" s="49"/>
       <c r="D32" s="35"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A33" s="55"/>
       <c r="B33" s="56"/>
       <c r="C33" s="56"/>
       <c r="D33" s="35"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A34" s="57"/>
       <c r="B34" s="58"/>
       <c r="C34" s="59"/>
       <c r="D34" s="35"/>
     </row>
-    <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="55"/>
       <c r="B35" s="56"/>
       <c r="C35" s="56"/>
@@ -2417,81 +2404,81 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="72">
+    <row r="36" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="73">
         <v>44328</v>
       </c>
-      <c r="B36" s="73"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="8"/>
       <c r="D36" s="35"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A37" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="46" t="s">
         <v>44</v>
-      </c>
-      <c r="B37" s="46" t="s">
-        <v>45</v>
       </c>
       <c r="C37" s="46">
         <v>0.5</v>
       </c>
       <c r="D37" s="35"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A38" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="48" t="s">
         <v>46</v>
-      </c>
-      <c r="B38" s="48" t="s">
-        <v>47</v>
       </c>
       <c r="C38" s="49">
         <v>6</v>
       </c>
       <c r="D38" s="35"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A39" s="45"/>
       <c r="B39" s="46"/>
       <c r="C39" s="46"/>
       <c r="D39" s="35"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A40" s="47"/>
       <c r="B40" s="48"/>
       <c r="C40" s="49"/>
       <c r="D40" s="35"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A41" s="45"/>
       <c r="B41" s="46"/>
       <c r="C41" s="46"/>
       <c r="D41" s="60"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A42" s="47"/>
       <c r="B42" s="48"/>
       <c r="C42" s="49"/>
       <c r="D42" s="35"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A43" s="50"/>
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
       <c r="D43" s="60"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A44" s="52"/>
       <c r="B44" s="53"/>
       <c r="C44" s="54"/>
       <c r="D44" s="35"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A45" s="55"/>
       <c r="B45" s="56"/>
       <c r="C45" s="56"/>
       <c r="D45" s="35"/>
     </row>
-    <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="57"/>
       <c r="B46" s="58"/>
       <c r="C46" s="59"/>
@@ -2500,17 +2487,17 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="74">
+    <row r="47" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="75">
         <v>44329</v>
       </c>
-      <c r="B47" s="75"/>
+      <c r="B47" s="76"/>
       <c r="C47" s="8"/>
       <c r="D47" s="35"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A48" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>10</v>
@@ -2520,9 +2507,9 @@
       </c>
       <c r="D48" s="35"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A49" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="46" t="s">
         <v>10</v>
@@ -2532,9 +2519,9 @@
       </c>
       <c r="D49" s="35"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A50" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="48" t="s">
         <v>22</v>
@@ -2544,49 +2531,49 @@
       </c>
       <c r="D50" s="35"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A51" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="46" t="s">
         <v>50</v>
-      </c>
-      <c r="B51" s="46" t="s">
-        <v>51</v>
       </c>
       <c r="C51" s="46">
         <v>6</v>
       </c>
       <c r="D51" s="35"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A52" s="47"/>
       <c r="B52" s="48"/>
       <c r="C52" s="49"/>
       <c r="D52" s="35"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A53" s="45"/>
       <c r="B53" s="46"/>
       <c r="C53" s="46"/>
       <c r="D53" s="35"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A54" s="47"/>
       <c r="B54" s="48"/>
       <c r="C54" s="49"/>
       <c r="D54" s="35"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A55" s="55"/>
       <c r="B55" s="56"/>
       <c r="C55" s="56"/>
       <c r="D55" s="35"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A56" s="57"/>
       <c r="B56" s="58"/>
       <c r="C56" s="59"/>
       <c r="D56" s="35"/>
     </row>
-    <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="55"/>
       <c r="B57" s="56"/>
       <c r="C57" s="56"/>
@@ -2595,17 +2582,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="72">
+    <row r="58" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="73">
         <v>44330</v>
       </c>
-      <c r="B58" s="73"/>
+      <c r="B58" s="74"/>
       <c r="C58" s="8"/>
       <c r="D58" s="35"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A59" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B59" s="46" t="s">
         <v>26</v>
@@ -2615,67 +2602,67 @@
       </c>
       <c r="D59" s="35"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A60" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60" s="48" t="s">
         <v>52</v>
-      </c>
-      <c r="B60" s="48" t="s">
-        <v>53</v>
       </c>
       <c r="C60" s="49">
         <v>3</v>
       </c>
       <c r="D60" s="35"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A61" s="45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B61" s="46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C61" s="46">
         <v>3</v>
       </c>
       <c r="D61" s="35"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A62" s="47"/>
       <c r="B62" s="48"/>
       <c r="C62" s="49"/>
       <c r="D62" s="35"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A63" s="45"/>
       <c r="B63" s="46"/>
       <c r="C63" s="46"/>
       <c r="D63" s="35"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A64" s="47"/>
       <c r="B64" s="48"/>
       <c r="C64" s="49"/>
       <c r="D64" s="35"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A65" s="50"/>
       <c r="B65" s="51"/>
       <c r="C65" s="51"/>
       <c r="D65" s="35"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A66" s="52"/>
       <c r="B66" s="53"/>
       <c r="C66" s="54"/>
       <c r="D66" s="35"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A67" s="55"/>
       <c r="B67" s="56"/>
       <c r="C67" s="56"/>
       <c r="D67" s="35"/>
     </row>
-    <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="57"/>
       <c r="B68" s="58"/>
       <c r="C68" s="59"/>
@@ -2684,69 +2671,69 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="74">
+    <row r="69" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="75">
         <v>44331</v>
       </c>
-      <c r="B69" s="75"/>
+      <c r="B69" s="76"/>
       <c r="C69" s="8"/>
       <c r="D69" s="35"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A70" s="47"/>
       <c r="B70" s="48"/>
       <c r="C70" s="49"/>
       <c r="D70" s="35"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A71" s="45"/>
       <c r="B71" s="46"/>
       <c r="C71" s="46"/>
       <c r="D71" s="35"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A72" s="47"/>
       <c r="B72" s="48"/>
       <c r="C72" s="49"/>
       <c r="D72" s="35"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A73" s="45"/>
       <c r="B73" s="46"/>
       <c r="C73" s="46"/>
       <c r="D73" s="35"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A74" s="47"/>
       <c r="B74" s="48"/>
       <c r="C74" s="49"/>
       <c r="D74" s="35"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A75" s="45"/>
       <c r="B75" s="46"/>
       <c r="C75" s="46"/>
       <c r="D75" s="35"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A76" s="47"/>
       <c r="B76" s="48"/>
       <c r="C76" s="49"/>
       <c r="D76" s="35"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A77" s="55"/>
       <c r="B77" s="56"/>
       <c r="C77" s="56"/>
       <c r="D77" s="35"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A78" s="57"/>
       <c r="B78" s="58"/>
       <c r="C78" s="59"/>
       <c r="D78" s="35"/>
     </row>
-    <row r="79" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="55"/>
       <c r="B79" s="56"/>
       <c r="C79" s="56"/>
@@ -2755,69 +2742,69 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="72">
+    <row r="80" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="73">
         <v>44332</v>
       </c>
-      <c r="B80" s="73"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="8"/>
       <c r="D80" s="35"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A81" s="45"/>
       <c r="B81" s="46"/>
       <c r="C81" s="46"/>
       <c r="D81" s="35"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A82" s="47"/>
       <c r="B82" s="48"/>
       <c r="C82" s="49"/>
       <c r="D82" s="35"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A83" s="45"/>
       <c r="B83" s="46"/>
       <c r="C83" s="46"/>
       <c r="D83" s="35"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A84" s="47"/>
       <c r="B84" s="48"/>
       <c r="C84" s="49"/>
       <c r="D84" s="35"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A85" s="45"/>
       <c r="B85" s="46"/>
       <c r="C85" s="46"/>
       <c r="D85" s="35"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A86" s="47"/>
       <c r="B86" s="48"/>
       <c r="C86" s="49"/>
       <c r="D86" s="35"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A87" s="50"/>
       <c r="B87" s="51"/>
       <c r="C87" s="51"/>
       <c r="D87" s="35"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A88" s="52"/>
       <c r="B88" s="53"/>
       <c r="C88" s="54"/>
       <c r="D88" s="35"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A89" s="55"/>
       <c r="B89" s="56"/>
       <c r="C89" s="56"/>
       <c r="D89" s="35"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A90" s="57"/>
       <c r="B90" s="58"/>
       <c r="C90" s="59"/>
@@ -2826,19 +2813,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A91" s="61"/>
       <c r="B91" s="61"/>
       <c r="C91" s="61"/>
       <c r="D91" s="35"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A92" s="62"/>
       <c r="B92" s="63"/>
       <c r="C92" s="63"/>
       <c r="D92" s="64"/>
     </row>
-    <row r="93" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="17" t="s">
         <v>27</v>
       </c>
@@ -2849,13 +2836,13 @@
       </c>
       <c r="D93" s="66"/>
     </row>
-    <row r="94" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="16.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A94" s="67"/>
       <c r="B94" s="68"/>
       <c r="C94" s="68"/>
       <c r="D94" s="35"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A95" s="62" t="s">
         <v>28</v>
       </c>
@@ -2863,37 +2850,37 @@
       <c r="C95" s="63"/>
       <c r="D95" s="21"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A96" s="69"/>
       <c r="B96" s="23"/>
       <c r="C96" s="23"/>
       <c r="D96" s="35"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A97" s="69"/>
       <c r="B97" s="23"/>
       <c r="C97" s="23"/>
       <c r="D97" s="35"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A98" s="67"/>
       <c r="B98" s="68"/>
       <c r="C98" s="68"/>
       <c r="D98" s="35"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A99" s="24"/>
       <c r="B99" s="24"/>
       <c r="C99" s="24"/>
       <c r="D99" s="35"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A100" s="35"/>
       <c r="B100" s="35"/>
       <c r="C100" s="35"/>
       <c r="D100" s="35"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="21"/>
@@ -2917,19 +2904,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0723633-256C-754A-A65B-B9FB88256DFB}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C62" activeCellId="7" sqref="C16 C18 C27:C28 C37 C48 C50 C59:C60 C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.1640625" customWidth="1"/>
+    <col min="1" max="1" width="53.19921875" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -2937,13 +2924,13 @@
       <c r="C1" s="1"/>
       <c r="D1" s="34"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="36"/>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A3" s="35"/>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
@@ -2951,7 +2938,7 @@
         <v>44333</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="s">
         <v>0</v>
       </c>
@@ -2961,7 +2948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>2</v>
       </c>
@@ -2971,7 +2958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
@@ -2979,19 +2966,19 @@
       <c r="C6" s="38"/>
       <c r="D6" s="35"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A7" s="38"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
       <c r="D7" s="35"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A8" s="35"/>
       <c r="B8" s="35"/>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A9" s="41" t="s">
         <v>4</v>
       </c>
@@ -2999,7 +2986,7 @@
       <c r="C9" s="42"/>
       <c r="D9" s="35"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -3007,19 +2994,19 @@
       <c r="C10" s="6"/>
       <c r="D10" s="35"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="35"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A12" s="35"/>
       <c r="B12" s="35"/>
       <c r="C12" s="35"/>
       <c r="D12" s="35"/>
     </row>
-    <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="43" t="s">
         <v>6</v>
       </c>
@@ -3031,27 +3018,27 @@
       </c>
       <c r="D13" s="44"/>
     </row>
-    <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72">
+    <row r="14" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="73">
         <v>44333</v>
       </c>
-      <c r="B14" s="73"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="8"/>
       <c r="D14" s="35"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A15" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C15" s="46">
         <v>3</v>
       </c>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A16" s="47" t="s">
         <v>34</v>
       </c>
@@ -3063,21 +3050,21 @@
       </c>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="C17" s="46">
         <v>2</v>
       </c>
       <c r="D17" s="35"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A18" s="47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="48" t="s">
         <v>22</v>
@@ -3087,37 +3074,37 @@
       </c>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A19" s="50"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A20" s="52"/>
       <c r="B20" s="53"/>
       <c r="C20" s="54"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A21" s="55"/>
       <c r="B21" s="56"/>
       <c r="C21" s="56"/>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A22" s="57"/>
       <c r="B22" s="58"/>
       <c r="C22" s="59"/>
       <c r="D22" s="35"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A23" s="55"/>
       <c r="B23" s="56"/>
       <c r="C23" s="56"/>
       <c r="D23" s="35"/>
     </row>
-    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="57"/>
       <c r="B24" s="58"/>
       <c r="C24" s="59"/>
@@ -3126,29 +3113,29 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="74">
+    <row r="25" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="75">
         <v>44334</v>
       </c>
-      <c r="B25" s="75"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="8"/>
       <c r="D25" s="35"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A26" s="47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="48" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C26" s="49">
         <v>1</v>
       </c>
       <c r="D26" s="35"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A27" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>10</v>
@@ -3158,144 +3145,144 @@
       </c>
       <c r="D27" s="35"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A28" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="49">
-        <v>0.66700000000000004</v>
+        <v>0.75</v>
       </c>
       <c r="D28" s="35"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A29" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C29" s="46">
         <v>4</v>
       </c>
       <c r="D29" s="35"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A30" s="47"/>
       <c r="B30" s="48"/>
       <c r="C30" s="49"/>
       <c r="D30" s="35"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A31" s="45"/>
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
       <c r="D31" s="35"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A32" s="47"/>
       <c r="B32" s="48"/>
       <c r="C32" s="49"/>
       <c r="D32" s="35"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A33" s="55"/>
       <c r="B33" s="56"/>
       <c r="C33" s="56"/>
       <c r="D33" s="35"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A34" s="57"/>
       <c r="B34" s="58"/>
       <c r="C34" s="59"/>
       <c r="D34" s="35"/>
     </row>
-    <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="55"/>
       <c r="B35" s="56"/>
       <c r="C35" s="56"/>
       <c r="D35" s="35">
         <f>SUM(C26:C35)</f>
-        <v>6.4169999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="72">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="73">
         <v>44335</v>
       </c>
-      <c r="B36" s="73"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="8"/>
       <c r="D36" s="35"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A37" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="46" t="s">
         <v>44</v>
-      </c>
-      <c r="B37" s="46" t="s">
-        <v>45</v>
       </c>
       <c r="C37" s="46">
         <v>0.5</v>
       </c>
       <c r="D37" s="35"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A38" s="70" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="48" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C38" s="49">
         <v>5.5</v>
       </c>
       <c r="D38" s="35"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A39" s="45"/>
       <c r="B39" s="46"/>
       <c r="C39" s="46"/>
       <c r="D39" s="35"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A40" s="47"/>
       <c r="B40" s="48"/>
       <c r="C40" s="49"/>
       <c r="D40" s="35"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A41" s="45"/>
       <c r="B41" s="46"/>
       <c r="C41" s="46"/>
       <c r="D41" s="60"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A42" s="47"/>
       <c r="B42" s="48"/>
       <c r="C42" s="49"/>
       <c r="D42" s="35"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A43" s="50"/>
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
       <c r="D43" s="60"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A44" s="52"/>
       <c r="B44" s="53"/>
       <c r="C44" s="54"/>
       <c r="D44" s="35"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A45" s="55"/>
       <c r="B45" s="56"/>
       <c r="C45" s="56"/>
       <c r="D45" s="35"/>
     </row>
-    <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="57"/>
       <c r="B46" s="58"/>
       <c r="C46" s="59"/>
@@ -3304,17 +3291,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="74">
+    <row r="47" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="75">
         <v>44336</v>
       </c>
-      <c r="B47" s="75"/>
+      <c r="B47" s="76"/>
       <c r="C47" s="8"/>
       <c r="D47" s="35"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A48" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>10</v>
@@ -3324,21 +3311,21 @@
       </c>
       <c r="D48" s="35"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A49" s="45" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B49" s="46" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C49" s="46">
         <v>6</v>
       </c>
       <c r="D49" s="35"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A50" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="48" t="s">
         <v>22</v>
@@ -3348,43 +3335,43 @@
       </c>
       <c r="D50" s="35"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A51" s="71"/>
       <c r="B51" s="46"/>
       <c r="C51" s="46"/>
       <c r="D51" s="35"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A52" s="47"/>
       <c r="B52" s="48"/>
       <c r="C52" s="49"/>
       <c r="D52" s="35"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A53" s="45"/>
       <c r="B53" s="46"/>
       <c r="C53" s="46"/>
       <c r="D53" s="35"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A54" s="47"/>
       <c r="B54" s="48"/>
       <c r="C54" s="49"/>
       <c r="D54" s="35"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A55" s="55"/>
       <c r="B55" s="56"/>
       <c r="C55" s="56"/>
       <c r="D55" s="35"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A56" s="57"/>
       <c r="B56" s="58"/>
       <c r="C56" s="59"/>
       <c r="D56" s="35"/>
     </row>
-    <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="55"/>
       <c r="B57" s="56"/>
       <c r="C57" s="56"/>
@@ -3393,17 +3380,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="72">
+    <row r="58" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="73">
         <v>44337</v>
       </c>
-      <c r="B58" s="73"/>
+      <c r="B58" s="74"/>
       <c r="C58" s="8"/>
       <c r="D58" s="35"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A59" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B59" s="46" t="s">
         <v>26</v>
@@ -3413,9 +3400,9 @@
       </c>
       <c r="D59" s="35"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A60" s="47" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B60" s="48" t="s">
         <v>22</v>
@@ -3425,150 +3412,150 @@
       </c>
       <c r="D60" s="35"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A61" s="45" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B61" s="46" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C61" s="46">
-        <v>0.66700000000000004</v>
+        <v>0.75</v>
       </c>
       <c r="D61" s="35"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A62" s="47" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B62" s="48" t="s">
         <v>26</v>
       </c>
       <c r="C62" s="49">
-        <v>0.33300000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="D62" s="35"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A63" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="46" t="s">
         <v>64</v>
-      </c>
-      <c r="B63" s="46" t="s">
-        <v>53</v>
       </c>
       <c r="C63" s="46">
         <v>1</v>
       </c>
       <c r="D63" s="35"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="76" t="s">
-        <v>65</v>
+    <row r="64" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A64" s="72" t="s">
+        <v>61</v>
       </c>
       <c r="B64" s="48" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C64" s="49">
         <v>3</v>
       </c>
       <c r="D64" s="35"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A65" s="50"/>
       <c r="B65" s="51"/>
       <c r="C65" s="51"/>
       <c r="D65" s="35"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A66" s="52"/>
       <c r="B66" s="53"/>
       <c r="C66" s="54"/>
       <c r="D66" s="35"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A67" s="55"/>
       <c r="B67" s="56"/>
       <c r="C67" s="56"/>
       <c r="D67" s="35"/>
     </row>
-    <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="57"/>
       <c r="B68" s="58"/>
       <c r="C68" s="59"/>
       <c r="D68" s="35">
         <f>SUM(C59:C68)</f>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="74">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="75">
         <v>44338</v>
       </c>
-      <c r="B69" s="75"/>
+      <c r="B69" s="76"/>
       <c r="C69" s="8"/>
       <c r="D69" s="35"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A70" s="47" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B70" s="48" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C70" s="49">
         <v>2</v>
       </c>
       <c r="D70" s="35"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A71" s="45"/>
       <c r="B71" s="46"/>
       <c r="C71" s="46"/>
       <c r="D71" s="35"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A72" s="47"/>
       <c r="B72" s="48"/>
       <c r="C72" s="49"/>
       <c r="D72" s="35"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A73" s="45"/>
       <c r="B73" s="46"/>
       <c r="C73" s="46"/>
       <c r="D73" s="35"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A74" s="47"/>
       <c r="B74" s="48"/>
       <c r="C74" s="49"/>
       <c r="D74" s="35"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A75" s="45"/>
       <c r="B75" s="46"/>
       <c r="C75" s="46"/>
       <c r="D75" s="35"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A76" s="47"/>
       <c r="B76" s="48"/>
       <c r="C76" s="49"/>
       <c r="D76" s="35"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A77" s="55"/>
       <c r="B77" s="56"/>
       <c r="C77" s="56"/>
       <c r="D77" s="35"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A78" s="57"/>
       <c r="B78" s="58"/>
       <c r="C78" s="59"/>
       <c r="D78" s="35"/>
     </row>
-    <row r="79" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="55"/>
       <c r="B79" s="56"/>
       <c r="C79" s="56"/>
@@ -3577,75 +3564,75 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="72">
+    <row r="80" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="73">
         <v>44339</v>
       </c>
-      <c r="B80" s="73"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="8"/>
       <c r="D80" s="35"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A81" s="45" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B81" s="46" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C81" s="46">
         <v>5</v>
       </c>
       <c r="D81" s="35"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A82" s="47"/>
       <c r="B82" s="48"/>
       <c r="C82" s="49"/>
       <c r="D82" s="35"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A83" s="45"/>
       <c r="B83" s="46"/>
       <c r="C83" s="46"/>
       <c r="D83" s="35"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A84" s="47"/>
       <c r="B84" s="48"/>
       <c r="C84" s="49"/>
       <c r="D84" s="35"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A85" s="45"/>
       <c r="B85" s="46"/>
       <c r="C85" s="46"/>
       <c r="D85" s="35"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A86" s="47"/>
       <c r="B86" s="48"/>
       <c r="C86" s="49"/>
       <c r="D86" s="35"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A87" s="50"/>
       <c r="B87" s="51"/>
       <c r="C87" s="51"/>
       <c r="D87" s="35"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A88" s="52"/>
       <c r="B88" s="53"/>
       <c r="C88" s="54"/>
       <c r="D88" s="35"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A89" s="55"/>
       <c r="B89" s="56"/>
       <c r="C89" s="56"/>
       <c r="D89" s="35"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A90" s="57"/>
       <c r="B90" s="58"/>
       <c r="C90" s="59"/>
@@ -3654,36 +3641,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A91" s="61"/>
       <c r="B91" s="61"/>
       <c r="C91" s="61"/>
       <c r="D91" s="35"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A92" s="62"/>
       <c r="B92" s="63"/>
       <c r="C92" s="63"/>
       <c r="D92" s="64"/>
     </row>
-    <row r="93" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B93" s="17"/>
       <c r="C93" s="65">
         <f>SUM(D24:D90)</f>
-        <v>40.417000000000002</v>
+        <v>40.75</v>
       </c>
       <c r="D93" s="66"/>
     </row>
-    <row r="94" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="16.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A94" s="67"/>
       <c r="B94" s="68"/>
       <c r="C94" s="68"/>
       <c r="D94" s="35"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A95" s="62" t="s">
         <v>28</v>
       </c>
@@ -3691,37 +3678,37 @@
       <c r="C95" s="63"/>
       <c r="D95" s="21"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A96" s="69"/>
       <c r="B96" s="23"/>
       <c r="C96" s="23"/>
       <c r="D96" s="35"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A97" s="69"/>
       <c r="B97" s="23"/>
       <c r="C97" s="23"/>
       <c r="D97" s="35"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A98" s="67"/>
       <c r="B98" s="68"/>
       <c r="C98" s="68"/>
       <c r="D98" s="35"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A99" s="24"/>
       <c r="B99" s="24"/>
       <c r="C99" s="24"/>
       <c r="D99" s="35"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A100" s="35"/>
       <c r="B100" s="35"/>
       <c r="C100" s="35"/>
       <c r="D100" s="35"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="21"/>

</xml_diff>

<commit_message>
update mitch work log
</commit_message>
<xml_diff>
--- a/personal-logs/mitch-harris/WorkLog_mh.xlsx
+++ b/personal-logs/mitch-harris/WorkLog_mh.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitch/data_labs/DATA599/w2020-data599-capstone-projects-ubc-udl/personal-logs/mitch-harris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08F09D3-A9C1-1847-9FA4-DB375B8F19C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C88529-3830-6C42-BD72-9B50E4F47D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="2" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="3" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
     <sheet name="Week 2" sheetId="2" r:id="rId2"/>
     <sheet name="Week 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Week 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="84">
   <si>
     <t>Master of Data Science Capstone Project - 2021</t>
   </si>
@@ -237,6 +238,57 @@
   </si>
   <si>
     <t>Build Flask App for serving models</t>
+  </si>
+  <si>
+    <t>LSTM research and testing</t>
+  </si>
+  <si>
+    <t>Presentation follow up</t>
+  </si>
+  <si>
+    <t>Prediction Pipeline creation</t>
+  </si>
+  <si>
+    <t>Pipeline discussion call</t>
+  </si>
+  <si>
+    <t>Implementing predictions with flask</t>
+  </si>
+  <si>
+    <t>Pipeline support for groupmate</t>
+  </si>
+  <si>
+    <t>Model Evaluation Notebook</t>
+  </si>
+  <si>
+    <t>Implementing predictions on loop without flask</t>
+  </si>
+  <si>
+    <t>Post sprint planning meeting</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Create model evaluation notebook template</t>
+  </si>
+  <si>
+    <t>Notebook template demo</t>
+  </si>
+  <si>
+    <t>Update model evaluation notebook template</t>
+  </si>
+  <si>
+    <t>Research LSTMs</t>
+  </si>
+  <si>
+    <t>Background research</t>
+  </si>
+  <si>
+    <t>Group call</t>
+  </si>
+  <si>
+    <t>Meeting with Nate to be updated on LSTM modifications</t>
   </si>
 </sst>
 </file>
@@ -592,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -836,6 +888,10 @@
       <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -852,7 +908,23 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
@@ -1427,11 +1499,11 @@
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72">
+      <c r="A14" s="73">
         <f>D3</f>
         <v>44319</v>
       </c>
-      <c r="B14" s="73"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1493,11 +1565,11 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="72">
+      <c r="A21" s="73">
         <f>A14+1</f>
         <v>44320</v>
       </c>
-      <c r="B21" s="73"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1570,11 +1642,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="72">
+      <c r="A29" s="73">
         <f>A21+1</f>
         <v>44321</v>
       </c>
-      <c r="B29" s="73"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1625,11 +1697,11 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="72">
+      <c r="A35" s="73">
         <f>A29+1</f>
         <v>44322</v>
       </c>
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1711,11 +1783,11 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="72">
+      <c r="A46" s="73">
         <f>A35+1</f>
         <v>44323</v>
       </c>
-      <c r="B46" s="73"/>
+      <c r="B46" s="74"/>
       <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1785,11 +1857,11 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="72">
+      <c r="A57" s="73">
         <f>A46+1</f>
         <v>44324</v>
       </c>
-      <c r="B57" s="73"/>
+      <c r="B57" s="74"/>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1847,11 +1919,11 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="72">
+      <c r="A68" s="73">
         <f>A57+1</f>
         <v>44325</v>
       </c>
-      <c r="B68" s="73"/>
+      <c r="B68" s="74"/>
       <c r="C68" s="8"/>
     </row>
     <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2107,8 +2179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27588B11-1EF5-1D41-B8BD-E638D371F0AF}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B64" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2222,10 +2294,10 @@
       <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72">
+      <c r="A14" s="73">
         <v>44326</v>
       </c>
-      <c r="B14" s="73"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="8"/>
       <c r="D14" s="35"/>
     </row>
@@ -2323,10 +2395,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="74">
+      <c r="A25" s="75">
         <v>44327</v>
       </c>
-      <c r="B25" s="75"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="8"/>
       <c r="D25" s="35"/>
     </row>
@@ -2418,10 +2490,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="72">
+      <c r="A36" s="73">
         <v>44328</v>
       </c>
-      <c r="B36" s="73"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="8"/>
       <c r="D36" s="35"/>
     </row>
@@ -2501,10 +2573,10 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="74">
+      <c r="A47" s="75">
         <v>44329</v>
       </c>
-      <c r="B47" s="75"/>
+      <c r="B47" s="76"/>
       <c r="C47" s="8"/>
       <c r="D47" s="35"/>
     </row>
@@ -2596,10 +2668,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="72">
+      <c r="A58" s="73">
         <v>44330</v>
       </c>
-      <c r="B58" s="73"/>
+      <c r="B58" s="74"/>
       <c r="C58" s="8"/>
       <c r="D58" s="35"/>
     </row>
@@ -2685,10 +2757,10 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="74">
+      <c r="A69" s="75">
         <v>44331</v>
       </c>
-      <c r="B69" s="75"/>
+      <c r="B69" s="76"/>
       <c r="C69" s="8"/>
       <c r="D69" s="35"/>
     </row>
@@ -2756,10 +2828,10 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="72">
+      <c r="A80" s="73">
         <v>44332</v>
       </c>
-      <c r="B80" s="73"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="8"/>
       <c r="D80" s="35"/>
     </row>
@@ -2917,8 +2989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0723633-256C-754A-A65B-B9FB88256DFB}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3032,10 +3104,10 @@
       <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72">
+      <c r="A14" s="73">
         <v>44333</v>
       </c>
-      <c r="B14" s="73"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="8"/>
       <c r="D14" s="35"/>
     </row>
@@ -3127,10 +3199,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="74">
+      <c r="A25" s="75">
         <v>44334</v>
       </c>
-      <c r="B25" s="75"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="8"/>
       <c r="D25" s="35"/>
     </row>
@@ -3222,10 +3294,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="72">
+      <c r="A36" s="73">
         <v>44335</v>
       </c>
-      <c r="B36" s="73"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="8"/>
       <c r="D36" s="35"/>
     </row>
@@ -3305,10 +3377,10 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="74">
+      <c r="A47" s="75">
         <v>44336</v>
       </c>
-      <c r="B47" s="75"/>
+      <c r="B47" s="76"/>
       <c r="C47" s="8"/>
       <c r="D47" s="35"/>
     </row>
@@ -3394,10 +3466,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="72">
+      <c r="A58" s="73">
         <v>44337</v>
       </c>
-      <c r="B58" s="73"/>
+      <c r="B58" s="74"/>
       <c r="C58" s="8"/>
       <c r="D58" s="35"/>
     </row>
@@ -3462,7 +3534,7 @@
       <c r="D63" s="35"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="76" t="s">
+      <c r="A64" s="72" t="s">
         <v>65</v>
       </c>
       <c r="B64" s="48" t="s">
@@ -3501,10 +3573,10 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="74">
+      <c r="A69" s="75">
         <v>44338</v>
       </c>
-      <c r="B69" s="75"/>
+      <c r="B69" s="76"/>
       <c r="C69" s="8"/>
       <c r="D69" s="35"/>
     </row>
@@ -3578,10 +3650,10 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="72">
+      <c r="A80" s="73">
         <v>44339</v>
       </c>
-      <c r="B80" s="73"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="8"/>
       <c r="D80" s="35"/>
     </row>
@@ -3674,6 +3746,842 @@
       <c r="C93" s="65">
         <f>SUM(D24:D90)</f>
         <v>40.417000000000002</v>
+      </c>
+      <c r="D93" s="66"/>
+    </row>
+    <row r="94" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="67"/>
+      <c r="B94" s="68"/>
+      <c r="C94" s="68"/>
+      <c r="D94" s="35"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" s="63"/>
+      <c r="C95" s="63"/>
+      <c r="D95" s="21"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="69"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="35"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="69"/>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="35"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="67"/>
+      <c r="B98" s="68"/>
+      <c r="C98" s="68"/>
+      <c r="D98" s="35"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="24"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="35"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="35"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="21"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A69:B69"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D472D863-B036-5B47-B942-D3CB1C88C09D}">
+  <dimension ref="A1:D101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="37">
+        <v>44340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="35"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="35"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="35"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="44"/>
+    </row>
+    <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="73">
+        <v>44340</v>
+      </c>
+      <c r="B14" s="74"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="35"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="46">
+        <v>4</v>
+      </c>
+      <c r="D15" s="35"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="49">
+        <v>0.75</v>
+      </c>
+      <c r="D16" s="35"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="45"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="35"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="47"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="45"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="55"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="57"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="35"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="55"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="35"/>
+    </row>
+    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="57"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="35">
+        <f>SUM(C15:C24)</f>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="75">
+        <v>44341</v>
+      </c>
+      <c r="B25" s="76"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="49">
+        <v>0.67</v>
+      </c>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="46">
+        <v>0.67</v>
+      </c>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="49">
+        <v>0.33</v>
+      </c>
+      <c r="D28" s="35"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="46">
+        <v>5</v>
+      </c>
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="47"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="45"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="35"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="47"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="35"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="79"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="35"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="57"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="35"/>
+    </row>
+    <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="55"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="35">
+        <f>SUM(C26:C35)</f>
+        <v>6.67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="73">
+        <v>44342</v>
+      </c>
+      <c r="B36" s="74"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="35"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="46">
+        <v>0.33</v>
+      </c>
+      <c r="D37" s="35"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="49">
+        <v>6</v>
+      </c>
+      <c r="D38" s="35"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="46">
+        <v>0.67</v>
+      </c>
+      <c r="D39" s="35"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="47"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="35"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="45"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="60"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="35"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="45"/>
+      <c r="B43" s="77"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="60"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="52"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="35"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="55"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="35"/>
+    </row>
+    <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="57"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="35">
+        <f>SUM(C37:C46)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="75">
+        <v>44343</v>
+      </c>
+      <c r="B47" s="76"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="35"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D48" s="35"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="46">
+        <v>2</v>
+      </c>
+      <c r="D49" s="35"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D50" s="35"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="46">
+        <v>2</v>
+      </c>
+      <c r="D51" s="35"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="49">
+        <v>2</v>
+      </c>
+      <c r="D52" s="35"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="D53" s="35"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="48"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="35"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="79"/>
+      <c r="B55" s="80"/>
+      <c r="C55" s="81"/>
+      <c r="D55" s="35"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="57"/>
+      <c r="B56" s="58"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="35"/>
+    </row>
+    <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="55"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="35">
+        <f>SUM(C48:C57)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="73">
+        <v>44344</v>
+      </c>
+      <c r="B58" s="74"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="35"/>
+    </row>
+    <row r="59" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="A59" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="D59" s="35"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" s="49">
+        <v>8</v>
+      </c>
+      <c r="D60" s="35"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" s="46">
+        <v>0.75</v>
+      </c>
+      <c r="D61" s="35"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="47"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="35"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="47"/>
+      <c r="B63" s="77"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="35"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="52"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="35"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="50"/>
+      <c r="B65" s="77"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="35"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="52"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="35"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="55"/>
+      <c r="B67" s="78"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="35"/>
+    </row>
+    <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="57"/>
+      <c r="B68" s="58"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="35">
+        <f>SUM(C59:C68)</f>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="75">
+        <v>44345</v>
+      </c>
+      <c r="B69" s="76"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="35"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C70" s="49">
+        <v>2</v>
+      </c>
+      <c r="D70" s="35"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="46">
+        <v>2</v>
+      </c>
+      <c r="D71" s="35"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B72" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D72" s="35"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="45"/>
+      <c r="B73" s="77"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="35"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="47"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="35"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="45"/>
+      <c r="B75" s="77"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="35"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="47"/>
+      <c r="B76" s="48"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="35"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="79"/>
+      <c r="B77" s="80"/>
+      <c r="C77" s="81"/>
+      <c r="D77" s="35"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="57"/>
+      <c r="B78" s="58"/>
+      <c r="C78" s="59"/>
+      <c r="D78" s="35"/>
+    </row>
+    <row r="79" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="55"/>
+      <c r="B79" s="78"/>
+      <c r="C79" s="56"/>
+      <c r="D79" s="35">
+        <f>SUM(C70:C79)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="73">
+        <v>44346</v>
+      </c>
+      <c r="B80" s="74"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="35"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B81" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81" s="46">
+        <v>0.75</v>
+      </c>
+      <c r="D81" s="35"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="47"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="35"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="45"/>
+      <c r="B83" s="77"/>
+      <c r="C83" s="46"/>
+      <c r="D83" s="35"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="47"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="35"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="45"/>
+      <c r="B85" s="77"/>
+      <c r="C85" s="46"/>
+      <c r="D85" s="35"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="47"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="35"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="45"/>
+      <c r="B87" s="77"/>
+      <c r="C87" s="46"/>
+      <c r="D87" s="35"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="52"/>
+      <c r="B88" s="53"/>
+      <c r="C88" s="54"/>
+      <c r="D88" s="35"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="55"/>
+      <c r="B89" s="78"/>
+      <c r="C89" s="56"/>
+      <c r="D89" s="35"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="57"/>
+      <c r="B90" s="58"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="35">
+        <f>SUM(C81:C89)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="61"/>
+      <c r="B91" s="61"/>
+      <c r="C91" s="61"/>
+      <c r="D91" s="35"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="62"/>
+      <c r="B92" s="63"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="64"/>
+    </row>
+    <row r="93" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93" s="17"/>
+      <c r="C93" s="65">
+        <f>SUM(D15:D90)</f>
+        <v>40.42</v>
       </c>
       <c r="D93" s="66"/>
     </row>

</xml_diff>

<commit_message>
update for week 5
</commit_message>
<xml_diff>
--- a/personal-logs/mitch-harris/WorkLog_mh.xlsx
+++ b/personal-logs/mitch-harris/WorkLog_mh.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitch/data_labs/DATA599/w2020-data599-capstone-projects-ubc-udl/personal-logs/mitch-harris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C88529-3830-6C42-BD72-9B50E4F47D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4671CF-06AD-E940-B6DF-7EEDD36B40C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="3" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="4" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
     <sheet name="Week 2" sheetId="2" r:id="rId2"/>
     <sheet name="Week 3" sheetId="3" r:id="rId3"/>
     <sheet name="Week 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Week 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="95">
   <si>
     <t>Master of Data Science Capstone Project - 2021</t>
   </si>
@@ -289,6 +290,39 @@
   </si>
   <si>
     <t>Meeting with Nate to be updated on LSTM modifications</t>
+  </si>
+  <si>
+    <t>Understand Influx</t>
+  </si>
+  <si>
+    <t>UDL meeting</t>
+  </si>
+  <si>
+    <t>Presentation run though</t>
+  </si>
+  <si>
+    <t>Understand Pipeline code</t>
+  </si>
+  <si>
+    <t>Stand up / Presentation practice</t>
+  </si>
+  <si>
+    <t>Learn Influx</t>
+  </si>
+  <si>
+    <t>Write test env pipeline</t>
+  </si>
+  <si>
+    <t>Create Test env</t>
+  </si>
+  <si>
+    <t>Test env set up with influx</t>
+  </si>
+  <si>
+    <t>Test Env set up and PR</t>
+  </si>
+  <si>
+    <t>Learn/Understand Influx</t>
   </si>
 </sst>
 </file>
@@ -892,6 +926,26 @@
       <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -906,26 +960,6 @@
     </xf>
     <xf numFmtId="16" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1499,11 +1533,11 @@
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73">
+      <c r="A14" s="78">
         <f>D3</f>
         <v>44319</v>
       </c>
-      <c r="B14" s="74"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1565,11 +1599,11 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73">
+      <c r="A21" s="78">
         <f>A14+1</f>
         <v>44320</v>
       </c>
-      <c r="B21" s="74"/>
+      <c r="B21" s="79"/>
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1642,11 +1676,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="73">
+      <c r="A29" s="78">
         <f>A21+1</f>
         <v>44321</v>
       </c>
-      <c r="B29" s="74"/>
+      <c r="B29" s="79"/>
       <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1697,11 +1731,11 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="73">
+      <c r="A35" s="78">
         <f>A29+1</f>
         <v>44322</v>
       </c>
-      <c r="B35" s="74"/>
+      <c r="B35" s="79"/>
       <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1783,11 +1817,11 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="73">
+      <c r="A46" s="78">
         <f>A35+1</f>
         <v>44323</v>
       </c>
-      <c r="B46" s="74"/>
+      <c r="B46" s="79"/>
       <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1857,11 +1891,11 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="73">
+      <c r="A57" s="78">
         <f>A46+1</f>
         <v>44324</v>
       </c>
-      <c r="B57" s="74"/>
+      <c r="B57" s="79"/>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1919,11 +1953,11 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="73">
+      <c r="A68" s="78">
         <f>A57+1</f>
         <v>44325</v>
       </c>
-      <c r="B68" s="74"/>
+      <c r="B68" s="79"/>
       <c r="C68" s="8"/>
     </row>
     <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2294,10 +2328,10 @@
       <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73">
+      <c r="A14" s="78">
         <v>44326</v>
       </c>
-      <c r="B14" s="74"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="8"/>
       <c r="D14" s="35"/>
     </row>
@@ -2395,10 +2429,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="75">
+      <c r="A25" s="80">
         <v>44327</v>
       </c>
-      <c r="B25" s="76"/>
+      <c r="B25" s="81"/>
       <c r="C25" s="8"/>
       <c r="D25" s="35"/>
     </row>
@@ -2490,10 +2524,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="73">
+      <c r="A36" s="78">
         <v>44328</v>
       </c>
-      <c r="B36" s="74"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="8"/>
       <c r="D36" s="35"/>
     </row>
@@ -2573,10 +2607,10 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="75">
+      <c r="A47" s="80">
         <v>44329</v>
       </c>
-      <c r="B47" s="76"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="8"/>
       <c r="D47" s="35"/>
     </row>
@@ -2668,10 +2702,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="73">
+      <c r="A58" s="78">
         <v>44330</v>
       </c>
-      <c r="B58" s="74"/>
+      <c r="B58" s="79"/>
       <c r="C58" s="8"/>
       <c r="D58" s="35"/>
     </row>
@@ -2757,10 +2791,10 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="75">
+      <c r="A69" s="80">
         <v>44331</v>
       </c>
-      <c r="B69" s="76"/>
+      <c r="B69" s="81"/>
       <c r="C69" s="8"/>
       <c r="D69" s="35"/>
     </row>
@@ -2828,10 +2862,10 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="73">
+      <c r="A80" s="78">
         <v>44332</v>
       </c>
-      <c r="B80" s="74"/>
+      <c r="B80" s="79"/>
       <c r="C80" s="8"/>
       <c r="D80" s="35"/>
     </row>
@@ -3104,10 +3138,10 @@
       <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73">
+      <c r="A14" s="78">
         <v>44333</v>
       </c>
-      <c r="B14" s="74"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="8"/>
       <c r="D14" s="35"/>
     </row>
@@ -3199,10 +3233,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="75">
+      <c r="A25" s="80">
         <v>44334</v>
       </c>
-      <c r="B25" s="76"/>
+      <c r="B25" s="81"/>
       <c r="C25" s="8"/>
       <c r="D25" s="35"/>
     </row>
@@ -3294,10 +3328,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="73">
+      <c r="A36" s="78">
         <v>44335</v>
       </c>
-      <c r="B36" s="74"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="8"/>
       <c r="D36" s="35"/>
     </row>
@@ -3377,10 +3411,10 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="75">
+      <c r="A47" s="80">
         <v>44336</v>
       </c>
-      <c r="B47" s="76"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="8"/>
       <c r="D47" s="35"/>
     </row>
@@ -3466,10 +3500,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="73">
+      <c r="A58" s="78">
         <v>44337</v>
       </c>
-      <c r="B58" s="74"/>
+      <c r="B58" s="79"/>
       <c r="C58" s="8"/>
       <c r="D58" s="35"/>
     </row>
@@ -3573,10 +3607,10 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="75">
+      <c r="A69" s="80">
         <v>44338</v>
       </c>
-      <c r="B69" s="76"/>
+      <c r="B69" s="81"/>
       <c r="C69" s="8"/>
       <c r="D69" s="35"/>
     </row>
@@ -3650,10 +3684,10 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="73">
+      <c r="A80" s="78">
         <v>44339</v>
       </c>
-      <c r="B80" s="74"/>
+      <c r="B80" s="79"/>
       <c r="C80" s="8"/>
       <c r="D80" s="35"/>
     </row>
@@ -3817,8 +3851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D472D863-B036-5B47-B942-D3CB1C88C09D}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3932,10 +3966,10 @@
       <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73">
+      <c r="A14" s="78">
         <v>44340</v>
       </c>
-      <c r="B14" s="74"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="8"/>
       <c r="D14" s="35"/>
     </row>
@@ -3943,7 +3977,7 @@
       <c r="A15" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="73" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="46">
@@ -3965,7 +3999,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="45"/>
-      <c r="B17" s="77"/>
+      <c r="B17" s="73"/>
       <c r="C17" s="46"/>
       <c r="D17" s="35"/>
     </row>
@@ -3977,7 +4011,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="45"/>
-      <c r="B19" s="77"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="46"/>
       <c r="D19" s="35"/>
     </row>
@@ -3989,7 +4023,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="55"/>
-      <c r="B21" s="78"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="56"/>
       <c r="D21" s="35"/>
     </row>
@@ -4001,7 +4035,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="55"/>
-      <c r="B23" s="78"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="56"/>
       <c r="D23" s="35"/>
     </row>
@@ -4015,10 +4049,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="75">
+      <c r="A25" s="80">
         <v>44341</v>
       </c>
-      <c r="B25" s="76"/>
+      <c r="B25" s="81"/>
       <c r="C25" s="8"/>
       <c r="D25" s="35"/>
     </row>
@@ -4038,7 +4072,7 @@
       <c r="A27" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="46">
@@ -4062,7 +4096,7 @@
       <c r="A29" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="77" t="s">
+      <c r="B29" s="73" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="46">
@@ -4078,7 +4112,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="45"/>
-      <c r="B31" s="77"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="46"/>
       <c r="D31" s="35"/>
     </row>
@@ -4089,9 +4123,9 @@
       <c r="D32" s="35"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="79"/>
-      <c r="B33" s="80"/>
-      <c r="C33" s="81"/>
+      <c r="A33" s="75"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="77"/>
       <c r="D33" s="35"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -4102,7 +4136,7 @@
     </row>
     <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="55"/>
-      <c r="B35" s="78"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="56"/>
       <c r="D35" s="35">
         <f>SUM(C26:C35)</f>
@@ -4110,10 +4144,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="73">
+      <c r="A36" s="78">
         <v>44342</v>
       </c>
-      <c r="B36" s="74"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="8"/>
       <c r="D36" s="35"/>
     </row>
@@ -4121,7 +4155,7 @@
       <c r="A37" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="77" t="s">
+      <c r="B37" s="73" t="s">
         <v>45</v>
       </c>
       <c r="C37" s="46">
@@ -4145,7 +4179,7 @@
       <c r="A39" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="77" t="s">
+      <c r="B39" s="73" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="46">
@@ -4161,7 +4195,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="45"/>
-      <c r="B41" s="77"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="46"/>
       <c r="D41" s="60"/>
     </row>
@@ -4173,7 +4207,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="45"/>
-      <c r="B43" s="77"/>
+      <c r="B43" s="73"/>
       <c r="C43" s="46"/>
       <c r="D43" s="60"/>
     </row>
@@ -4185,7 +4219,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="55"/>
-      <c r="B45" s="78"/>
+      <c r="B45" s="74"/>
       <c r="C45" s="56"/>
       <c r="D45" s="35"/>
     </row>
@@ -4199,10 +4233,10 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="75">
+      <c r="A47" s="80">
         <v>44343</v>
       </c>
-      <c r="B47" s="76"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="8"/>
       <c r="D47" s="35"/>
     </row>
@@ -4222,7 +4256,7 @@
       <c r="A49" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="77" t="s">
+      <c r="B49" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="46">
@@ -4246,7 +4280,7 @@
       <c r="A51" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="77" t="s">
+      <c r="B51" s="73" t="s">
         <v>53</v>
       </c>
       <c r="C51" s="46">
@@ -4270,7 +4304,7 @@
       <c r="A53" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="77" t="s">
+      <c r="B53" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C53" s="46">
@@ -4287,9 +4321,9 @@
       <c r="D54" s="35"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="79"/>
-      <c r="B55" s="80"/>
-      <c r="C55" s="81"/>
+      <c r="A55" s="75"/>
+      <c r="B55" s="76"/>
+      <c r="C55" s="77"/>
       <c r="D55" s="35"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -4300,7 +4334,7 @@
     </row>
     <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="55"/>
-      <c r="B57" s="78"/>
+      <c r="B57" s="74"/>
       <c r="C57" s="56"/>
       <c r="D57" s="35">
         <f>SUM(C48:C57)</f>
@@ -4308,10 +4342,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="73">
+      <c r="A58" s="78">
         <v>44344</v>
       </c>
-      <c r="B58" s="74"/>
+      <c r="B58" s="79"/>
       <c r="C58" s="8"/>
       <c r="D58" s="35"/>
     </row>
@@ -4319,7 +4353,7 @@
       <c r="A59" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B59" s="77" t="s">
+      <c r="B59" s="73" t="s">
         <v>26</v>
       </c>
       <c r="C59" s="46">
@@ -4343,7 +4377,7 @@
       <c r="A61" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="77" t="s">
+      <c r="B61" s="73" t="s">
         <v>26</v>
       </c>
       <c r="C61" s="46">
@@ -4359,7 +4393,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="47"/>
-      <c r="B63" s="77"/>
+      <c r="B63" s="73"/>
       <c r="C63" s="46"/>
       <c r="D63" s="35"/>
     </row>
@@ -4371,7 +4405,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="50"/>
-      <c r="B65" s="77"/>
+      <c r="B65" s="73"/>
       <c r="C65" s="46"/>
       <c r="D65" s="35"/>
     </row>
@@ -4383,7 +4417,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="55"/>
-      <c r="B67" s="78"/>
+      <c r="B67" s="74"/>
       <c r="C67" s="56"/>
       <c r="D67" s="35"/>
     </row>
@@ -4397,10 +4431,10 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="75">
+      <c r="A69" s="80">
         <v>44345</v>
       </c>
-      <c r="B69" s="76"/>
+      <c r="B69" s="81"/>
       <c r="C69" s="8"/>
       <c r="D69" s="35"/>
     </row>
@@ -4420,7 +4454,7 @@
       <c r="A71" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="B71" s="77" t="s">
+      <c r="B71" s="73" t="s">
         <v>81</v>
       </c>
       <c r="C71" s="46">
@@ -4442,7 +4476,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="45"/>
-      <c r="B73" s="77"/>
+      <c r="B73" s="73"/>
       <c r="C73" s="46"/>
       <c r="D73" s="35"/>
     </row>
@@ -4454,7 +4488,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="45"/>
-      <c r="B75" s="77"/>
+      <c r="B75" s="73"/>
       <c r="C75" s="46"/>
       <c r="D75" s="35"/>
     </row>
@@ -4465,9 +4499,9 @@
       <c r="D76" s="35"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="79"/>
-      <c r="B77" s="80"/>
-      <c r="C77" s="81"/>
+      <c r="A77" s="75"/>
+      <c r="B77" s="76"/>
+      <c r="C77" s="77"/>
       <c r="D77" s="35"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -4478,7 +4512,7 @@
     </row>
     <row r="79" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="55"/>
-      <c r="B79" s="78"/>
+      <c r="B79" s="74"/>
       <c r="C79" s="56"/>
       <c r="D79" s="35">
         <f>SUM(C70:C79)</f>
@@ -4486,10 +4520,10 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="73">
+      <c r="A80" s="78">
         <v>44346</v>
       </c>
-      <c r="B80" s="74"/>
+      <c r="B80" s="79"/>
       <c r="C80" s="8"/>
       <c r="D80" s="35"/>
     </row>
@@ -4497,7 +4531,7 @@
       <c r="A81" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="B81" s="77" t="s">
+      <c r="B81" s="73" t="s">
         <v>26</v>
       </c>
       <c r="C81" s="46">
@@ -4513,7 +4547,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="45"/>
-      <c r="B83" s="77"/>
+      <c r="B83" s="73"/>
       <c r="C83" s="46"/>
       <c r="D83" s="35"/>
     </row>
@@ -4525,7 +4559,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="45"/>
-      <c r="B85" s="77"/>
+      <c r="B85" s="73"/>
       <c r="C85" s="46"/>
       <c r="D85" s="35"/>
     </row>
@@ -4537,7 +4571,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="45"/>
-      <c r="B87" s="77"/>
+      <c r="B87" s="73"/>
       <c r="C87" s="46"/>
       <c r="D87" s="35"/>
     </row>
@@ -4549,7 +4583,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="55"/>
-      <c r="B89" s="78"/>
+      <c r="B89" s="74"/>
       <c r="C89" s="56"/>
       <c r="D89" s="35"/>
     </row>
@@ -4582,6 +4616,818 @@
       <c r="C93" s="65">
         <f>SUM(D15:D90)</f>
         <v>40.42</v>
+      </c>
+      <c r="D93" s="66"/>
+    </row>
+    <row r="94" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="67"/>
+      <c r="B94" s="68"/>
+      <c r="C94" s="68"/>
+      <c r="D94" s="35"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" s="63"/>
+      <c r="C95" s="63"/>
+      <c r="D95" s="21"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="69"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="35"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="69"/>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="35"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="67"/>
+      <c r="B98" s="68"/>
+      <c r="C98" s="68"/>
+      <c r="D98" s="35"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="24"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="35"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="35"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="21"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A69:B69"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3017ED-B44A-2C41-8222-9F8375580B7F}">
+  <dimension ref="A1:D101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="37">
+        <v>44347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="35"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="35"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="35"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="44"/>
+    </row>
+    <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="78">
+        <v>44347</v>
+      </c>
+      <c r="B14" s="79"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="35"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="46">
+        <v>3</v>
+      </c>
+      <c r="D15" s="35"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="35"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="35"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="49">
+        <v>1</v>
+      </c>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="46">
+        <v>1</v>
+      </c>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="55"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="57"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="35"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="55"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="35"/>
+    </row>
+    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="57"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="35">
+        <f>SUM(C15:C24)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="80">
+        <v>44348</v>
+      </c>
+      <c r="B25" s="81"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="46">
+        <v>0.33</v>
+      </c>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="47"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="35"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="46">
+        <v>5</v>
+      </c>
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="47"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="45"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="35"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="47"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="35"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="75"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="35"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="57"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="35"/>
+    </row>
+    <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="55"/>
+      <c r="B35" s="74"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="35">
+        <f>SUM(C26:C35)</f>
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="78">
+        <v>44349</v>
+      </c>
+      <c r="B36" s="79"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="35"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="73" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="46">
+        <v>0.67</v>
+      </c>
+      <c r="D37" s="35"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="49">
+        <v>6</v>
+      </c>
+      <c r="D38" s="35"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="46">
+        <v>2</v>
+      </c>
+      <c r="D39" s="35"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="47"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="35"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="45"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="60"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="35"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="45"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="60"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="52"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="35"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="55"/>
+      <c r="B45" s="74"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="35"/>
+    </row>
+    <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="57"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="35">
+        <f>SUM(C37:C46)</f>
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="80">
+        <v>44350</v>
+      </c>
+      <c r="B47" s="81"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="35"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="D48" s="35"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="46">
+        <v>6</v>
+      </c>
+      <c r="D49" s="35"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="49">
+        <v>1</v>
+      </c>
+      <c r="D50" s="35"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="71"/>
+      <c r="B51" s="73"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="35"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="47"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="35"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="45"/>
+      <c r="B53" s="73"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="35"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="48"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="35"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="75"/>
+      <c r="B55" s="76"/>
+      <c r="C55" s="77"/>
+      <c r="D55" s="35"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="57"/>
+      <c r="B56" s="58"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="35"/>
+    </row>
+    <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="55"/>
+      <c r="B57" s="74"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="35">
+        <f>SUM(C48:C57)</f>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="78">
+        <v>44351</v>
+      </c>
+      <c r="B58" s="79"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="35"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="46">
+        <v>0.33</v>
+      </c>
+      <c r="D59" s="35"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" s="49">
+        <v>6</v>
+      </c>
+      <c r="D60" s="35"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B61" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="46">
+        <v>2</v>
+      </c>
+      <c r="D61" s="35"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="47"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="35"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="47"/>
+      <c r="B63" s="73"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="35"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="52"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="35"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="50"/>
+      <c r="B65" s="73"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="35"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="52"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="35"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="55"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="35"/>
+    </row>
+    <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="57"/>
+      <c r="B68" s="58"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="35">
+        <f>SUM(C59:C68)</f>
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="80">
+        <v>44352</v>
+      </c>
+      <c r="B69" s="81"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="35"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C70" s="49">
+        <v>5</v>
+      </c>
+      <c r="D70" s="35"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="45"/>
+      <c r="B71" s="73"/>
+      <c r="C71" s="46"/>
+      <c r="D71" s="35"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="47"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="35"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="45"/>
+      <c r="B73" s="73"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="35"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="47"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="35"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="45"/>
+      <c r="B75" s="73"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="35"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="47"/>
+      <c r="B76" s="48"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="35"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="75"/>
+      <c r="B77" s="76"/>
+      <c r="C77" s="77"/>
+      <c r="D77" s="35"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="57"/>
+      <c r="B78" s="58"/>
+      <c r="C78" s="59"/>
+      <c r="D78" s="35"/>
+    </row>
+    <row r="79" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="55"/>
+      <c r="B79" s="74"/>
+      <c r="C79" s="56"/>
+      <c r="D79" s="35">
+        <f>SUM(C70:C79)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="78">
+        <v>44353</v>
+      </c>
+      <c r="B80" s="79"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="35"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="45"/>
+      <c r="B81" s="73"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="35"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="47"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="35"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="45"/>
+      <c r="B83" s="73"/>
+      <c r="C83" s="46"/>
+      <c r="D83" s="35"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="47"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="35"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="45"/>
+      <c r="B85" s="73"/>
+      <c r="C85" s="46"/>
+      <c r="D85" s="35"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="47"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="35"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="45"/>
+      <c r="B87" s="73"/>
+      <c r="C87" s="46"/>
+      <c r="D87" s="35"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="52"/>
+      <c r="B88" s="53"/>
+      <c r="C88" s="54"/>
+      <c r="D88" s="35"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="55"/>
+      <c r="B89" s="74"/>
+      <c r="C89" s="56"/>
+      <c r="D89" s="35"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="57"/>
+      <c r="B90" s="58"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="35">
+        <f>SUM(C81:C89)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="61"/>
+      <c r="B91" s="61"/>
+      <c r="C91" s="61"/>
+      <c r="D91" s="35"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="62"/>
+      <c r="B92" s="63"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="64"/>
+    </row>
+    <row r="93" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93" s="17"/>
+      <c r="C93" s="65">
+        <f>SUM(D15:D90)</f>
+        <v>41.08</v>
       </c>
       <c r="D93" s="66"/>
     </row>

</xml_diff>

<commit_message>
add week 7 hours
</commit_message>
<xml_diff>
--- a/personal-logs/mitch-harris/WorkLog_mh.xlsx
+++ b/personal-logs/mitch-harris/WorkLog_mh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitch/data_labs/DATA599/w2020-data599-capstone-projects-ubc-udl/personal-logs/mitch-harris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CA4C8B-94DB-7449-838C-E58FDBC39160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFAB429-CE38-1846-B7A6-0AEB5AFF2A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="5" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="6" xr2:uid="{354C69BC-D109-8549-BEC8-BCAF6F8B45DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Week 4" sheetId="4" r:id="rId4"/>
     <sheet name="Week 5" sheetId="5" r:id="rId5"/>
     <sheet name="Week 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Week 7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="115">
   <si>
     <t>Master of Data Science Capstone Project - 2021</t>
   </si>
@@ -345,6 +346,45 @@
   </si>
   <si>
     <t xml:space="preserve">Create InfluxDB Dashboard Notifications </t>
+  </si>
+  <si>
+    <t>Finish Test Environment</t>
+  </si>
+  <si>
+    <t>Notebook runthrough call with Nate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Call with Ryan about notebook</t>
+  </si>
+  <si>
+    <t>Update Test Env</t>
+  </si>
+  <si>
+    <t>Stand up and follow up call with Ryan</t>
+  </si>
+  <si>
+    <t>Test Env Call with Nate</t>
+  </si>
+  <si>
+    <t>Integrate Updated Model Methodology</t>
+  </si>
+  <si>
+    <t>Update other files to match the test env notebook</t>
+  </si>
+  <si>
+    <t>Fix bugs in Test Env</t>
+  </si>
+  <si>
+    <t>Notebook call</t>
+  </si>
+  <si>
+    <t>Notebook debug call</t>
+  </si>
+  <si>
+    <t>Investigate bugs in test env notebook</t>
+  </si>
+  <si>
+    <t>Add delete logic to test env notebook and address other PR notes</t>
   </si>
 </sst>
 </file>
@@ -700,7 +740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -983,6 +1023,13 @@
     <xf numFmtId="16" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5521,8 +5568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFE7E91-47FD-F24D-81CB-0B88C88D733F}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6306,4 +6353,822 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925C15CE-786C-4947-A37F-D9DDD6CFBE6C}">
+  <dimension ref="A1:D101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="37">
+        <v>44361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="35"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="35"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="35"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="44"/>
+    </row>
+    <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="78">
+        <v>44361</v>
+      </c>
+      <c r="B14" s="79"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="35"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="35"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="35"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="46">
+        <v>8</v>
+      </c>
+      <c r="D17" s="35"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="47"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="45"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="55"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="57"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="35"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="55"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="35"/>
+    </row>
+    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="57"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="35">
+        <f>SUM(C15:C24)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="80">
+        <v>44362</v>
+      </c>
+      <c r="B25" s="81"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="46">
+        <v>0.33</v>
+      </c>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="83" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="84">
+        <v>0.25</v>
+      </c>
+      <c r="D28" s="82"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="51">
+        <v>10</v>
+      </c>
+      <c r="D29" s="82"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="47"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="45"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="35"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="47"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="35"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="75"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="35"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="57"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="35"/>
+    </row>
+    <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="55"/>
+      <c r="B35" s="74"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="35">
+        <f>SUM(C26:C35)</f>
+        <v>11.08</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="78">
+        <v>44363</v>
+      </c>
+      <c r="B36" s="79"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="35"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="46">
+        <v>9</v>
+      </c>
+      <c r="D37" s="35"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D38" s="35"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="46">
+        <v>1</v>
+      </c>
+      <c r="D39" s="35"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="47"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="35"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="45"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="60"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="35"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="45"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="60"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="52"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="35"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="55"/>
+      <c r="B45" s="74"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="35"/>
+    </row>
+    <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="57"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="35">
+        <f>SUM(C37:C46)</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="80">
+        <v>44364</v>
+      </c>
+      <c r="B47" s="81"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="35"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D48" s="35"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="46">
+        <v>6</v>
+      </c>
+      <c r="D49" s="35"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="D50" s="35"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="71"/>
+      <c r="B51" s="73"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="35"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="47"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="35"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="45"/>
+      <c r="B53" s="73"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="35"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="48"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="35"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="75"/>
+      <c r="B55" s="76"/>
+      <c r="C55" s="77"/>
+      <c r="D55" s="35"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="57"/>
+      <c r="B56" s="58"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="35"/>
+    </row>
+    <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="55"/>
+      <c r="B57" s="74"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="35">
+        <f>SUM(C48:C57)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="78">
+        <v>44365</v>
+      </c>
+      <c r="B58" s="79"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="35"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="46">
+        <v>0.25</v>
+      </c>
+      <c r="D59" s="35"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" s="49">
+        <v>5</v>
+      </c>
+      <c r="D60" s="35"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="45"/>
+      <c r="B61" s="73"/>
+      <c r="C61" s="46"/>
+      <c r="D61" s="35"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="47"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="35"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="47"/>
+      <c r="B63" s="73"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="35"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="52"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="35"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="50"/>
+      <c r="B65" s="73"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="35"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="52"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="35"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="55"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="35"/>
+    </row>
+    <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="57"/>
+      <c r="B68" s="58"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="35">
+        <f>SUM(C59:C68)</f>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="80">
+        <v>44366</v>
+      </c>
+      <c r="B69" s="81"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="35"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="49">
+        <v>0.75</v>
+      </c>
+      <c r="D70" s="35"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="D71" s="35"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B72" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C72" s="49">
+        <v>3.5</v>
+      </c>
+      <c r="D72" s="35"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="45"/>
+      <c r="B73" s="73"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="35"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="47"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="35"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="45"/>
+      <c r="B75" s="73"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="35"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="47"/>
+      <c r="B76" s="48"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="35"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="75"/>
+      <c r="B77" s="76"/>
+      <c r="C77" s="77"/>
+      <c r="D77" s="35"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="57"/>
+      <c r="B78" s="58"/>
+      <c r="C78" s="59"/>
+      <c r="D78" s="35"/>
+    </row>
+    <row r="79" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="55"/>
+      <c r="B79" s="74"/>
+      <c r="C79" s="56"/>
+      <c r="D79" s="35">
+        <f>SUM(C70:C79)</f>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="78">
+        <v>44367</v>
+      </c>
+      <c r="B80" s="79"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="35"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="B81" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C81" s="46">
+        <v>2</v>
+      </c>
+      <c r="D81" s="35"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="47"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="35"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="45"/>
+      <c r="B83" s="73"/>
+      <c r="C83" s="46"/>
+      <c r="D83" s="35"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="47"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="35"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="45"/>
+      <c r="B85" s="73"/>
+      <c r="C85" s="46"/>
+      <c r="D85" s="35"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="47"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="35"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="45"/>
+      <c r="B87" s="73"/>
+      <c r="C87" s="46"/>
+      <c r="D87" s="35"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="52"/>
+      <c r="B88" s="53"/>
+      <c r="C88" s="54"/>
+      <c r="D88" s="35"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="55"/>
+      <c r="B89" s="74"/>
+      <c r="C89" s="56"/>
+      <c r="D89" s="35"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="57"/>
+      <c r="B90" s="58"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="35">
+        <f>SUM(C81:C89)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="61"/>
+      <c r="B91" s="61"/>
+      <c r="C91" s="61"/>
+      <c r="D91" s="35"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="62"/>
+      <c r="B92" s="63"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="64"/>
+    </row>
+    <row r="93" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93" s="17"/>
+      <c r="C93" s="65">
+        <f>SUM(D15:D90)</f>
+        <v>49.58</v>
+      </c>
+      <c r="D93" s="66"/>
+    </row>
+    <row r="94" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="67"/>
+      <c r="B94" s="68"/>
+      <c r="C94" s="68"/>
+      <c r="D94" s="35"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" s="63"/>
+      <c r="C95" s="63"/>
+      <c r="D95" s="21"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="69"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="35"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="69"/>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="35"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="67"/>
+      <c r="B98" s="68"/>
+      <c r="C98" s="68"/>
+      <c r="D98" s="35"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="24"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="35"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="35"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="21"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A69:B69"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>